<commit_message>
mudança para ler extrato nubank
</commit_message>
<xml_diff>
--- a/extrato_classificado.xlsx
+++ b/extrato_classificado.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,13 +450,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-02-01</v>
+        <v>2025-09-01</v>
       </c>
       <c r="B2" t="str">
-        <v>Transferência Pix recebida EURIVAL BATISTA NUNES</v>
+        <v>Transferência Recebida - Fred Williams de Oliveira Lima Junior - •••.938.792-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 19569491-2</v>
       </c>
       <c r="C2" t="str">
-        <v>EURIVAL BATISTA NUNES</v>
+        <v>Fred Williams de Oliveira Lima Junior</v>
       </c>
       <c r="D2" t="str">
         <v/>
@@ -465,7 +465,7 @@
         <v>credito</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>1591.35</v>
       </c>
       <c r="G2" t="str">
         <v>Transferências</v>
@@ -477,30 +477,30 @@
         <v>PIX</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>NU PAGAMENTOS</v>
       </c>
       <c r="K2" t="str">
         <v/>
       </c>
       <c r="L2" t="str">
-        <v>Transferência PIX recebida de terceiro; nome favorecido diferente do titular, classificada por heurística (palavra Pix e nome não associado)</v>
+        <v>Transferência recebida via PIX, favorecido não parece o titular, classificado como transferência a terceiros.</v>
       </c>
       <c r="M2">
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="N2" t="str">
-        <v>7efc3c0639fef864152bb8f8c745a273</v>
+        <v>68b58bc1-95c1-43af-8dd9-6e79ffa7981c</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-02-01</v>
+        <v>2025-09-01</v>
       </c>
       <c r="B3" t="str">
-        <v>Pagamento com QR Pix AUTO POSTO GK LTDA</v>
+        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
       </c>
       <c r="C3" t="str">
-        <v>AUTO POSTO GK LTDA</v>
+        <v>Arthur Andrade Nunes</v>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -509,13 +509,13 @@
         <v>debito</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>1591.35</v>
       </c>
       <c r="G3" t="str">
-        <v>Transporte</v>
+        <v>Transferências</v>
       </c>
       <c r="H3" t="str">
-        <v>Combustível/Estacionamento</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I3" t="str">
         <v>PIX</v>
@@ -524,159 +524,159 @@
         <v/>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>MERCADO PAGO IP LTDA.</v>
       </c>
       <c r="L3" t="str">
-        <v>Estabelecimento com POSTO identificado em dicionário de palavras-chave para combustível</v>
+        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M3">
-        <v>0.92</v>
+        <v>0.65</v>
       </c>
       <c r="N3" t="str">
-        <v>2ab1a7ff4a809fd4185ea546e1837ab7</v>
+        <v>68b59f38-3b11-43af-8ce2-6619375c06fb</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-02-01</v>
+        <v>2025-09-03</v>
       </c>
       <c r="B4" t="str">
-        <v>Pagamento com QR Pix RAIA DROGASIL SA</v>
+        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
       </c>
       <c r="C4" t="str">
-        <v>RAIA DROGASIL SA</v>
+        <v>Adisraely C Andrade Silva</v>
       </c>
       <c r="D4" t="str">
         <v/>
       </c>
       <c r="E4" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="F4">
-        <v>24.93</v>
+        <v>100</v>
       </c>
       <c r="G4" t="str">
-        <v>Saúde</v>
+        <v>Transferências</v>
       </c>
       <c r="H4" t="str">
-        <v>Farmácia</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I4" t="str">
         <v>PIX</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>BCO DO BRASIL S.A.</v>
       </c>
       <c r="K4" t="str">
         <v/>
       </c>
       <c r="L4" t="str">
-        <v>Estabelecimento farmacêutico reconhecido (palavra-chave DROGASIL); alta confiança</v>
+        <v>Transferência recebida via PIX de terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M4">
-        <v>0.98</v>
+        <v>0.65</v>
       </c>
       <c r="N4" t="str">
-        <v>aa6356fcd505ea6d158b5ee13e12e74f</v>
+        <v>68b8e7c0-884a-4b9d-ba6a-8769217c588c</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-02-03</v>
+        <v>2025-09-04</v>
       </c>
       <c r="B5" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência enviada pelo Pix - IGOR VINICIUS GOMES DE OLIVEIRA - •••.869.528-•• - BCO BRADESCO S.A. (0237) Agência: 909 Conta: 3460-6</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>Igor Vinicius Gomes de Oliveira</v>
       </c>
       <c r="D5" t="str">
         <v/>
       </c>
       <c r="E5" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F5">
-        <v>2.51</v>
+        <v>74.25</v>
       </c>
       <c r="G5" t="str">
-        <v>Renda</v>
+        <v>Transferências</v>
       </c>
       <c r="H5" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I5" t="str">
-        <v/>
+        <v>PIX</v>
       </c>
       <c r="J5" t="str">
         <v/>
       </c>
       <c r="K5" t="str">
-        <v/>
+        <v>BCO BRADESCO S.A.</v>
       </c>
       <c r="L5" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M5">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="N5" t="str">
-        <v>d0eebd61f10cd20fc95afdeb7bff5f0d</v>
+        <v>68b97efe-de9f-4fde-adc8-550b21ec0f0f</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-02-03</v>
+        <v>2025-09-05</v>
       </c>
       <c r="B6" t="str">
-        <v>Transferência Pix enviada Arthur Andrade Nunes</v>
+        <v>Transferência de saldo NuInvest</v>
       </c>
       <c r="C6" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>NuInvest</v>
       </c>
       <c r="D6" t="str">
         <v/>
       </c>
       <c r="E6" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="F6">
-        <v>322.62</v>
+        <v>1.98</v>
       </c>
       <c r="G6" t="str">
-        <v>Transferências</v>
+        <v>Renda</v>
       </c>
       <c r="H6" t="str">
-        <v>Transferência a terceiros</v>
+        <v>Rendimentos/Investimentos</v>
       </c>
       <c r="I6" t="str">
-        <v>PIX</v>
+        <v>TEF</v>
       </c>
       <c r="J6" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="K6" t="str">
         <v/>
       </c>
       <c r="L6" t="str">
-        <v>PIX enviada para terceiro (nome diferente do titular)</v>
+        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
       </c>
       <c r="M6">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="N6" t="str">
-        <v>d915d43d23ffa4bf24b7e3a08a883b2a</v>
+        <v>68bad327-eb76-4d9b-ab6b-8272708e7058</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-02-03</v>
+        <v>2025-09-06</v>
       </c>
       <c r="B7" t="str">
-        <v>Aplicação em fundo de investimento</v>
+        <v>Compra no débito via NuPay - Uber</v>
       </c>
       <c r="C7" t="str">
-        <v/>
+        <v>Uber</v>
       </c>
       <c r="D7" t="str">
         <v/>
@@ -685,16 +685,16 @@
         <v>debito</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>21.93</v>
       </c>
       <c r="G7" t="str">
-        <v>Investimentos</v>
+        <v>Transporte</v>
       </c>
       <c r="H7" t="str">
-        <v>Aporte</v>
+        <v>App</v>
       </c>
       <c r="I7" t="str">
-        <v/>
+        <v>cartão débito</v>
       </c>
       <c r="J7" t="str">
         <v/>
@@ -703,24 +703,24 @@
         <v/>
       </c>
       <c r="L7" t="str">
-        <v>Aplicação em fundo de investimento; termo 'aplicação' reconhecido como aporte</v>
+        <v>Descrição contém 'Uber' (palavra-chave de transporte app).</v>
       </c>
       <c r="M7">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="N7" t="str">
-        <v>30247e2c2f77a8e34a33544fd5902d41</v>
+        <v>68bc748b-bb47-48ae-9674-c299fd4451d2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-02-04</v>
+        <v>2025-09-11</v>
       </c>
       <c r="B8" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência de saldo NuInvest</v>
       </c>
       <c r="C8" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -729,7 +729,7 @@
         <v>credito</v>
       </c>
       <c r="F8">
-        <v>2.35</v>
+        <v>0.09</v>
       </c>
       <c r="G8" t="str">
         <v>Renda</v>
@@ -738,33 +738,33 @@
         <v>Rendimentos/Investimentos</v>
       </c>
       <c r="I8" t="str">
-        <v/>
+        <v>TEF</v>
       </c>
       <c r="J8" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="K8" t="str">
         <v/>
       </c>
       <c r="L8" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
       </c>
       <c r="M8">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="N8" t="str">
-        <v>0a5c501a153783812128596b3bae2e3d</v>
+        <v>68c2bc51-c9a5-4f97-8310-ec55c7f13e5b</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-02-05</v>
+        <v>2025-09-12</v>
       </c>
       <c r="B9" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência de saldo NuInvest</v>
       </c>
       <c r="C9" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -773,7 +773,7 @@
         <v>credito</v>
       </c>
       <c r="F9">
-        <v>2.35</v>
+        <v>0.82</v>
       </c>
       <c r="G9" t="str">
         <v>Renda</v>
@@ -782,77 +782,77 @@
         <v>Rendimentos/Investimentos</v>
       </c>
       <c r="I9" t="str">
-        <v/>
+        <v>TEF</v>
       </c>
       <c r="J9" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="K9" t="str">
         <v/>
       </c>
       <c r="L9" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
       </c>
       <c r="M9">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="N9" t="str">
-        <v>c6067aca9bf048ae1c62405a6ca9f31a</v>
+        <v>68c40e37-2615-4d5c-884c-c2b6eb593755</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-02-05</v>
+        <v>2025-09-12</v>
       </c>
       <c r="B10" t="str">
-        <v>Transferência Pix enviada Caio Tiago Rodrigues Dos Santos</v>
+        <v>Transferência de saldo NuInvest</v>
       </c>
       <c r="C10" t="str">
-        <v>Caio Tiago Rodrigues Dos Santos</v>
+        <v>NuInvest</v>
       </c>
       <c r="D10" t="str">
         <v/>
       </c>
       <c r="E10" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="F10">
-        <v>65</v>
+        <v>1.2</v>
       </c>
       <c r="G10" t="str">
-        <v>Transferências</v>
+        <v>Renda</v>
       </c>
       <c r="H10" t="str">
-        <v>Transferência a terceiros</v>
+        <v>Rendimentos/Investimentos</v>
       </c>
       <c r="I10" t="str">
-        <v>PIX</v>
+        <v>TEF</v>
       </c>
       <c r="J10" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="K10" t="str">
         <v/>
       </c>
       <c r="L10" t="str">
-        <v>PIX enviada para terceiro (nome diferente do titular)</v>
+        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
       </c>
       <c r="M10">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="N10" t="str">
-        <v>ee2375c1c8bf4b79b2f2ea497cee92ab</v>
+        <v>68c40e37-d692-4c74-a8f0-7da6a7004150</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-02-06</v>
+        <v>2025-09-12</v>
       </c>
       <c r="B11" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência de saldo NuInvest</v>
       </c>
       <c r="C11" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="D11" t="str">
         <v/>
@@ -861,7 +861,7 @@
         <v>credito</v>
       </c>
       <c r="F11">
-        <v>2.32</v>
+        <v>0.74</v>
       </c>
       <c r="G11" t="str">
         <v>Renda</v>
@@ -870,33 +870,33 @@
         <v>Rendimentos/Investimentos</v>
       </c>
       <c r="I11" t="str">
-        <v/>
+        <v>TEF</v>
       </c>
       <c r="J11" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="K11" t="str">
         <v/>
       </c>
       <c r="L11" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
       </c>
       <c r="M11">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="N11" t="str">
-        <v>b2996f20302c04fbc28cbbd8fcf85df3</v>
+        <v>68c40e38-45e2-44a3-9d29-aba78f835f0d</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-02-07</v>
+        <v>2025-09-12</v>
       </c>
       <c r="B12" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência de saldo NuInvest</v>
       </c>
       <c r="C12" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="D12" t="str">
         <v/>
@@ -905,7 +905,7 @@
         <v>credito</v>
       </c>
       <c r="F12">
-        <v>2.32</v>
+        <v>3.24</v>
       </c>
       <c r="G12" t="str">
         <v>Renda</v>
@@ -914,51 +914,51 @@
         <v>Rendimentos/Investimentos</v>
       </c>
       <c r="I12" t="str">
-        <v/>
+        <v>TEF</v>
       </c>
       <c r="J12" t="str">
-        <v/>
+        <v>NuInvest</v>
       </c>
       <c r="K12" t="str">
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
       </c>
       <c r="M12">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="N12" t="str">
-        <v>12d0adea4adefae7ef7c39dc678bb1dc</v>
+        <v>68c40e3a-fc05-41ec-88b8-b8f30506276c</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-02-09</v>
+        <v>2025-09-17</v>
       </c>
       <c r="B13" t="str">
-        <v>Transferência Pix recebida EURIVAL BATISTA NUNES</v>
+        <v>Compra no débito - MINI KALZONE</v>
       </c>
       <c r="C13" t="str">
-        <v>EURIVAL BATISTA NUNES</v>
+        <v>MINI KALZONE</v>
       </c>
       <c r="D13" t="str">
         <v/>
       </c>
       <c r="E13" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F13">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G13" t="str">
-        <v>Transferências</v>
+        <v>Alimentação</v>
       </c>
       <c r="H13" t="str">
-        <v>Transferência a terceiros</v>
+        <v>Restaurante</v>
       </c>
       <c r="I13" t="str">
-        <v>PIX</v>
+        <v>cartão débito</v>
       </c>
       <c r="J13" t="str">
         <v/>
@@ -967,24 +967,24 @@
         <v/>
       </c>
       <c r="L13" t="str">
-        <v>Transferência PIX recebida de terceiro; nome favorecido diferente do titular, classificada por heurística (palavra Pix e nome não associado)</v>
+        <v>Estabelecimento sugere restaurante/fast-food.</v>
       </c>
       <c r="M13">
-        <v>0.85</v>
+        <v>0.92</v>
       </c>
       <c r="N13" t="str">
-        <v>d7c0e4f092525fa230244e30a5cc0fa0</v>
+        <v>68cb0900-49ea-4f71-b890-bf64f7d0a9eb</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-02-10</v>
+        <v>2025-09-22</v>
       </c>
       <c r="B14" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência recebida pelo Pix - EURIVAL BATISTA NUNES - •••.965.195-•• - BCO DO BRASIL S.A. (0001) Agência: 5752 Conta: 6897-7</v>
       </c>
       <c r="C14" t="str">
-        <v/>
+        <v>Eurival Batista Nunes</v>
       </c>
       <c r="D14" t="str">
         <v/>
@@ -993,57 +993,57 @@
         <v>credito</v>
       </c>
       <c r="F14">
-        <v>2.33</v>
+        <v>300</v>
       </c>
       <c r="G14" t="str">
-        <v>Renda</v>
+        <v>Transferências</v>
       </c>
       <c r="H14" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I14" t="str">
-        <v/>
+        <v>PIX</v>
       </c>
       <c r="J14" t="str">
-        <v/>
+        <v>BCO DO BRASIL S.A.</v>
       </c>
       <c r="K14" t="str">
         <v/>
       </c>
       <c r="L14" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência recebida via PIX de terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M14">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="N14" t="str">
-        <v>e1e15634dad570fca285ca64c9515b51</v>
+        <v>68d13fcb-b5f5-48f4-ab48-671f3d23d658</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-02-10</v>
+        <v>2025-09-22</v>
       </c>
       <c r="B15" t="str">
-        <v>Transferência Pix recebida LIVEPIX</v>
+        <v>Transferência enviada pelo Pix - ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA - 34.075.739/0001-84 - ITAÚ UNIBANCO S.A. (0341) Agência: 459 Conta: 33230-0</v>
       </c>
       <c r="C15" t="str">
-        <v>LIVEPIX</v>
+        <v>ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA</v>
       </c>
       <c r="D15" t="str">
-        <v/>
+        <v>34.075.739/0001-84</v>
       </c>
       <c r="E15" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F15">
-        <v>34.2</v>
+        <v>149</v>
       </c>
       <c r="G15" t="str">
-        <v>Transferências</v>
+        <v>Educação</v>
       </c>
       <c r="H15" t="str">
-        <v>Transferência a terceiros</v>
+        <v>Mensalidade</v>
       </c>
       <c r="I15" t="str">
         <v>PIX</v>
@@ -1052,42 +1052,42 @@
         <v/>
       </c>
       <c r="K15" t="str">
-        <v/>
+        <v>ITAÚ UNIBANCO S.A.</v>
       </c>
       <c r="L15" t="str">
-        <v>Transferência PIX recebida de terceiro; estabelecimento diferente do titular, classificado como transferência a terceiros</v>
+        <v>Nome e CNPJ correspondem a instituição de ensino. Palavra-chave 'Escola'.</v>
       </c>
       <c r="M15">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="N15" t="str">
-        <v>2cf77197beea905b0e6e40d6be64d21d</v>
+        <v>68d14071-2832-47e2-8b42-f2d9ed2b46bb</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2025-02-10</v>
+        <v>2025-09-22</v>
       </c>
       <c r="B16" t="str">
-        <v>Transferência Pix enviada Kalleb Guimaraes Ferreira</v>
+        <v>Transferência enviada pelo Pix - ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA - 34.075.739/0001-84 - ITAÚ UNIBANCO S.A. (0341) Agência: 459 Conta: 33230-0</v>
       </c>
       <c r="C16" t="str">
-        <v>Kalleb Guimaraes Ferreira</v>
+        <v>ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA</v>
       </c>
       <c r="D16" t="str">
-        <v/>
+        <v>34.075.739/0001-84</v>
       </c>
       <c r="E16" t="str">
         <v>debito</v>
       </c>
       <c r="F16">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="G16" t="str">
-        <v>Transferências</v>
+        <v>Educação</v>
       </c>
       <c r="H16" t="str">
-        <v>Transferência a terceiros</v>
+        <v>Mensalidade</v>
       </c>
       <c r="I16" t="str">
         <v>PIX</v>
@@ -1096,68 +1096,68 @@
         <v/>
       </c>
       <c r="K16" t="str">
-        <v/>
+        <v>ITAÚ UNIBANCO S.A.</v>
       </c>
       <c r="L16" t="str">
-        <v>PIX enviada para terceiro (nome diferente do titular)</v>
+        <v>Nome e CNPJ correspondem a instituição de ensino. Palavra-chave 'Escola'. Possível duplicidade de pagamento.</v>
       </c>
       <c r="M16">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="N16" t="str">
-        <v>9b29262e340ad93f6d8092b2bb8013fe</v>
+        <v>68d17dba-ac23-4282-8808-cd3377be4ab3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2025-02-10</v>
+        <v>2025-09-26</v>
       </c>
       <c r="B17" t="str">
-        <v>Pagamento com QR Pix MOURA ALIMENTOS</v>
+        <v>Transferência recebida pelo Pix - Arthur Andrade Nunes - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
       </c>
       <c r="C17" t="str">
-        <v>MOURA ALIMENTOS</v>
+        <v>Arthur Andrade Nunes</v>
       </c>
       <c r="D17" t="str">
         <v/>
       </c>
       <c r="E17" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>757.56</v>
       </c>
       <c r="G17" t="str">
-        <v>Alimentação</v>
+        <v>Transferências</v>
       </c>
       <c r="H17" t="str">
-        <v>Supermercado</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I17" t="str">
         <v>PIX</v>
       </c>
       <c r="J17" t="str">
-        <v/>
+        <v>MERCADO PAGO IP LTDA.</v>
       </c>
       <c r="K17" t="str">
         <v/>
       </c>
       <c r="L17" t="str">
-        <v>Palavra 'ALIMENTOS' sugere compra em supermercado; heurística e ausência de termo restaurante/lanchonete/delivery</v>
+        <v>Transferência recebida via PIX, favorecido não parece o titular, classificado como transferência a terceiros.</v>
       </c>
       <c r="M17">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="N17" t="str">
-        <v>36e16b77959a162b976ce70381ff48e0</v>
+        <v>68d713ea-986d-45fe-842d-975fc51a17f0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2025-02-11</v>
+        <v>2025-09-26</v>
       </c>
       <c r="B18" t="str">
-        <v>Rendimentos</v>
+        <v>Pagamento de fatura</v>
       </c>
       <c r="C18" t="str">
         <v/>
@@ -1166,19 +1166,19 @@
         <v/>
       </c>
       <c r="E18" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F18">
-        <v>2.34</v>
+        <v>757.56</v>
       </c>
       <c r="G18" t="str">
-        <v>Renda</v>
+        <v>Serviços financeiros</v>
       </c>
       <c r="H18" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Cartão – Pagamento de fatura</v>
       </c>
       <c r="I18" t="str">
-        <v/>
+        <v>cartão crédito</v>
       </c>
       <c r="J18" t="str">
         <v/>
@@ -1187,24 +1187,24 @@
         <v/>
       </c>
       <c r="L18" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Pagamento de fatura de cartão, não computar como gasto novo (liquidação). Excluir do total de saídas.</v>
       </c>
       <c r="M18">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="N18" t="str">
-        <v>acebeb8efc4afc9ad619b519eb06ba2d</v>
+        <v>68d713ff-5ac6-4d47-9674-c135d7aeeb31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2025-02-12</v>
+        <v>2025-09-27</v>
       </c>
       <c r="B19" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência recebida pelo Pix - JOHN LUCAS MAGNAVITA DE ALMEIDA - •••.924.005-•• - BANCO INTER (0077) Agência: 1 Conta: 36925596-8</v>
       </c>
       <c r="C19" t="str">
-        <v/>
+        <v>John Lucas Magnavita de Almeida</v>
       </c>
       <c r="D19" t="str">
         <v/>
@@ -1213,60 +1213,60 @@
         <v>credito</v>
       </c>
       <c r="F19">
-        <v>2.34</v>
+        <v>500</v>
       </c>
       <c r="G19" t="str">
-        <v>Renda</v>
+        <v>Transferências</v>
       </c>
       <c r="H19" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I19" t="str">
-        <v/>
+        <v>PIX</v>
       </c>
       <c r="J19" t="str">
-        <v/>
+        <v>BANCO INTER</v>
       </c>
       <c r="K19" t="str">
         <v/>
       </c>
       <c r="L19" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência recebida via PIX de terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M19">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="N19" t="str">
-        <v>bdd8afdbe2ddcae33a265d070447907f</v>
+        <v>68d81c64-7ae7-4337-a9d0-c8ca9268abb1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2025-02-13</v>
+        <v>2025-09-27</v>
       </c>
       <c r="B20" t="str">
-        <v>Rendimentos</v>
+        <v>Compra no débito via NuPay - Uber</v>
       </c>
       <c r="C20" t="str">
-        <v/>
+        <v>Uber</v>
       </c>
       <c r="D20" t="str">
         <v/>
       </c>
       <c r="E20" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F20">
-        <v>2.35</v>
+        <v>13.23</v>
       </c>
       <c r="G20" t="str">
-        <v>Renda</v>
+        <v>Transporte</v>
       </c>
       <c r="H20" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>App</v>
       </c>
       <c r="I20" t="str">
-        <v/>
+        <v>cartão débito</v>
       </c>
       <c r="J20" t="str">
         <v/>
@@ -1275,24 +1275,24 @@
         <v/>
       </c>
       <c r="L20" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Descrição contém 'Uber' (palavra-chave de transporte app).</v>
       </c>
       <c r="M20">
         <v>0.95</v>
       </c>
       <c r="N20" t="str">
-        <v>309ebe39af3c0a31c3209fa27120c241</v>
+        <v>68d86970-7e36-4f39-9c0b-7c35eb994be3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2025-02-13</v>
+        <v>2025-09-27</v>
       </c>
       <c r="B21" t="str">
-        <v>Aplicação em fundo de investimento</v>
+        <v>Compra no débito - JeronimoFlorianop</v>
       </c>
       <c r="C21" t="str">
-        <v/>
+        <v>JeronimoFlorianop</v>
       </c>
       <c r="D21" t="str">
         <v/>
@@ -1301,16 +1301,16 @@
         <v>debito</v>
       </c>
       <c r="F21">
-        <v>900</v>
+        <v>57</v>
       </c>
       <c r="G21" t="str">
-        <v>Investimentos</v>
+        <v>Alimentação</v>
       </c>
       <c r="H21" t="str">
-        <v>Aporte</v>
+        <v>Restaurante</v>
       </c>
       <c r="I21" t="str">
-        <v/>
+        <v>cartão débito</v>
       </c>
       <c r="J21" t="str">
         <v/>
@@ -1319,86 +1319,86 @@
         <v/>
       </c>
       <c r="L21" t="str">
-        <v>Aplicação em fundo de investimento; termo 'aplicação' reconhecido como aporte</v>
+        <v>Estabelecimento aparenta ser restaurante de fast food. Pela convenção da marca Jeronimo, classificado como Alimentação/Restaurante.</v>
       </c>
       <c r="M21">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="N21" t="str">
-        <v>954c030dd9d302ff4db529be773be422</v>
+        <v>68d87576-526a-4e24-995d-a214ec00ee05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>2025-02-14</v>
+        <v>2025-09-27</v>
       </c>
       <c r="B22" t="str">
-        <v>Rendimentos</v>
+        <v>Transferência enviada pelo Pix - Miriã dos Reis Almeida - •••.758.569-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 41331813-8</v>
       </c>
       <c r="C22" t="str">
-        <v/>
+        <v>Miriã dos Reis Almeida</v>
       </c>
       <c r="D22" t="str">
         <v/>
       </c>
       <c r="E22" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F22">
-        <v>2.35</v>
+        <v>13</v>
       </c>
       <c r="G22" t="str">
-        <v>Renda</v>
+        <v>Transferências</v>
       </c>
       <c r="H22" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Transferência a terceiros</v>
       </c>
       <c r="I22" t="str">
-        <v/>
+        <v>PIX</v>
       </c>
       <c r="J22" t="str">
         <v/>
       </c>
       <c r="K22" t="str">
-        <v/>
+        <v>NU PAGAMENTOS</v>
       </c>
       <c r="L22" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M22">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="N22" t="str">
-        <v>fe9fea569c01df7fb6d5e2976d08a0e0</v>
+        <v>68d88096-1f88-4ea5-a1d1-6800f7a58635</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>2025-02-17</v>
+        <v>2025-09-28</v>
       </c>
       <c r="B23" t="str">
-        <v>Rendimentos</v>
+        <v>Compra no débito via NuPay - Uber</v>
       </c>
       <c r="C23" t="str">
-        <v/>
+        <v>Uber</v>
       </c>
       <c r="D23" t="str">
         <v/>
       </c>
       <c r="E23" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="F23">
-        <v>1.99</v>
+        <v>9.43</v>
       </c>
       <c r="G23" t="str">
-        <v>Renda</v>
+        <v>Transporte</v>
       </c>
       <c r="H23" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>App</v>
       </c>
       <c r="I23" t="str">
-        <v/>
+        <v>cartão débito</v>
       </c>
       <c r="J23" t="str">
         <v/>
@@ -1407,24 +1407,24 @@
         <v/>
       </c>
       <c r="L23" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
+        <v>Descrição contém 'Uber' (palavra-chave de transporte app).</v>
       </c>
       <c r="M23">
         <v>0.95</v>
       </c>
       <c r="N23" t="str">
-        <v>66f27e49dbba1a8933d87faeffe9be1f</v>
+        <v>68d9c2ae-9c68-4cde-aa22-740d26f291d6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>2025-02-17</v>
+        <v>2025-09-28</v>
       </c>
       <c r="B24" t="str">
-        <v>Investimento em CDB</v>
+        <v>Compra no débito - OUTBACK STEAKHOUSE</v>
       </c>
       <c r="C24" t="str">
-        <v/>
+        <v>OUTBACK STEAKHOUSE</v>
       </c>
       <c r="D24" t="str">
         <v/>
@@ -1433,16 +1433,16 @@
         <v>debito</v>
       </c>
       <c r="F24">
-        <v>3000</v>
+        <v>204.62</v>
       </c>
       <c r="G24" t="str">
-        <v>Investimentos</v>
+        <v>Alimentação</v>
       </c>
       <c r="H24" t="str">
-        <v>Aporte</v>
+        <v>Restaurante</v>
       </c>
       <c r="I24" t="str">
-        <v/>
+        <v>cartão débito</v>
       </c>
       <c r="J24" t="str">
         <v/>
@@ -1451,24 +1451,24 @@
         <v/>
       </c>
       <c r="L24" t="str">
-        <v>Investimento em CDB; termo 'investimento' e padrão reconhecido</v>
+        <v>Nome do estabelecimento é de restaurante, classificado como Alimentação/Restaurante.</v>
       </c>
       <c r="M24">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="N24" t="str">
-        <v>523576c1940bfe83aac3f140b322336f</v>
+        <v>68d9dbad-042c-46d0-aec6-430cf5ffef54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>2025-02-17</v>
+        <v>2025-09-29</v>
       </c>
       <c r="B25" t="str">
-        <v>Transferência Pix enviada Michell Richard Cunha dos Prazeres</v>
+        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
       </c>
       <c r="C25" t="str">
-        <v>Michell Richard Cunha dos Prazeres</v>
+        <v>Arthur Andrade Nunes</v>
       </c>
       <c r="D25" t="str">
         <v/>
@@ -1477,7 +1477,7 @@
         <v>debito</v>
       </c>
       <c r="F25">
-        <v>200</v>
+        <v>206.61</v>
       </c>
       <c r="G25" t="str">
         <v>Transferências</v>
@@ -1492,505 +1492,21 @@
         <v/>
       </c>
       <c r="K25" t="str">
-        <v/>
+        <v>MERCADO PAGO IP LTDA.</v>
       </c>
       <c r="L25" t="str">
-        <v>PIX enviada para terceiro (nome diferente do titular)</v>
+        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
       </c>
       <c r="M25">
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="N25" t="str">
-        <v>373058b09fcf5e09b6c0cce5eacff85d</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>2025-02-18</v>
-      </c>
-      <c r="B26" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C26" t="str">
-        <v/>
-      </c>
-      <c r="D26" t="str">
-        <v/>
-      </c>
-      <c r="E26" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F26">
-        <v>0.71</v>
-      </c>
-      <c r="G26" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H26" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I26" t="str">
-        <v/>
-      </c>
-      <c r="J26" t="str">
-        <v/>
-      </c>
-      <c r="K26" t="str">
-        <v/>
-      </c>
-      <c r="L26" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M26">
-        <v>0.95</v>
-      </c>
-      <c r="N26" t="str">
-        <v>95a0aaf403c209bb9e132f4d550ab6d2</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>2025-02-18</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Transferência Pix recebida EURIVAL BATISTA NUNES</v>
-      </c>
-      <c r="C27" t="str">
-        <v>EURIVAL BATISTA NUNES</v>
-      </c>
-      <c r="D27" t="str">
-        <v/>
-      </c>
-      <c r="E27" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F27">
-        <v>50</v>
-      </c>
-      <c r="G27" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H27" t="str">
-        <v>Transferência a terceiros</v>
-      </c>
-      <c r="I27" t="str">
-        <v>PIX</v>
-      </c>
-      <c r="J27" t="str">
-        <v/>
-      </c>
-      <c r="K27" t="str">
-        <v/>
-      </c>
-      <c r="L27" t="str">
-        <v>Transferência PIX recebida de terceiro; nome favorecido diferente do titular, classificada por heurística (palavra Pix e nome não associado)</v>
-      </c>
-      <c r="M27">
-        <v>0.85</v>
-      </c>
-      <c r="N27" t="str">
-        <v>b27745fd88582a3347e871c7daadeafe</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>2025-02-18</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Pagamento com QR Pix POSTO GONCALVES LTDA</v>
-      </c>
-      <c r="C28" t="str">
-        <v>POSTO GONCALVES LTDA</v>
-      </c>
-      <c r="D28" t="str">
-        <v/>
-      </c>
-      <c r="E28" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F28">
-        <v>50</v>
-      </c>
-      <c r="G28" t="str">
-        <v>Transporte</v>
-      </c>
-      <c r="H28" t="str">
-        <v>Combustível/Estacionamento</v>
-      </c>
-      <c r="I28" t="str">
-        <v>PIX</v>
-      </c>
-      <c r="J28" t="str">
-        <v/>
-      </c>
-      <c r="K28" t="str">
-        <v/>
-      </c>
-      <c r="L28" t="str">
-        <v>Estabelecimento com POSTO identificado em dicionário de palavras-chave para combustível</v>
-      </c>
-      <c r="M28">
-        <v>0.92</v>
-      </c>
-      <c r="N28" t="str">
-        <v>b11fdda59cda5978fbb7f1f84b439f18</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>2025-02-19</v>
-      </c>
-      <c r="B29" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C29" t="str">
-        <v/>
-      </c>
-      <c r="D29" t="str">
-        <v/>
-      </c>
-      <c r="E29" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F29">
-        <v>0.71</v>
-      </c>
-      <c r="G29" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H29" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I29" t="str">
-        <v/>
-      </c>
-      <c r="J29" t="str">
-        <v/>
-      </c>
-      <c r="K29" t="str">
-        <v/>
-      </c>
-      <c r="L29" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M29">
-        <v>0.95</v>
-      </c>
-      <c r="N29" t="str">
-        <v>7933e66f5c7115760a0325382a4fb628</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>2025-02-20</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C30" t="str">
-        <v/>
-      </c>
-      <c r="D30" t="str">
-        <v/>
-      </c>
-      <c r="E30" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F30">
-        <v>0.71</v>
-      </c>
-      <c r="G30" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H30" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I30" t="str">
-        <v/>
-      </c>
-      <c r="J30" t="str">
-        <v/>
-      </c>
-      <c r="K30" t="str">
-        <v/>
-      </c>
-      <c r="L30" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M30">
-        <v>0.95</v>
-      </c>
-      <c r="N30" t="str">
-        <v>ae1e2a5638b1748c282cdf326e8ec032</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>2025-02-21</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C31" t="str">
-        <v/>
-      </c>
-      <c r="D31" t="str">
-        <v/>
-      </c>
-      <c r="E31" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F31">
-        <v>0.7</v>
-      </c>
-      <c r="G31" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H31" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I31" t="str">
-        <v/>
-      </c>
-      <c r="J31" t="str">
-        <v/>
-      </c>
-      <c r="K31" t="str">
-        <v/>
-      </c>
-      <c r="L31" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M31">
-        <v>0.95</v>
-      </c>
-      <c r="N31" t="str">
-        <v>d0d9a3bbe3c04bcc9e2368cd437f005d</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>2025-02-24</v>
-      </c>
-      <c r="B32" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C32" t="str">
-        <v/>
-      </c>
-      <c r="D32" t="str">
-        <v/>
-      </c>
-      <c r="E32" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F32">
-        <v>2.36</v>
-      </c>
-      <c r="G32" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H32" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I32" t="str">
-        <v/>
-      </c>
-      <c r="J32" t="str">
-        <v/>
-      </c>
-      <c r="K32" t="str">
-        <v/>
-      </c>
-      <c r="L32" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M32">
-        <v>0.95</v>
-      </c>
-      <c r="N32" t="str">
-        <v>79b05ee700e1f70dd52277adce5bb24d</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>2025-02-25</v>
-      </c>
-      <c r="B33" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C33" t="str">
-        <v/>
-      </c>
-      <c r="D33" t="str">
-        <v/>
-      </c>
-      <c r="E33" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F33">
-        <v>0.72</v>
-      </c>
-      <c r="G33" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H33" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I33" t="str">
-        <v/>
-      </c>
-      <c r="J33" t="str">
-        <v/>
-      </c>
-      <c r="K33" t="str">
-        <v/>
-      </c>
-      <c r="L33" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M33">
-        <v>0.95</v>
-      </c>
-      <c r="N33" t="str">
-        <v>b73904fa5124a52681f3642a85ece8ce</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>2025-02-26</v>
-      </c>
-      <c r="B34" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C34" t="str">
-        <v/>
-      </c>
-      <c r="D34" t="str">
-        <v/>
-      </c>
-      <c r="E34" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F34">
-        <v>0.71</v>
-      </c>
-      <c r="G34" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H34" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I34" t="str">
-        <v/>
-      </c>
-      <c r="J34" t="str">
-        <v/>
-      </c>
-      <c r="K34" t="str">
-        <v/>
-      </c>
-      <c r="L34" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M34">
-        <v>0.95</v>
-      </c>
-      <c r="N34" t="str">
-        <v>384b6d9928cdc168310da8a1f2d53f30</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>2025-02-27</v>
-      </c>
-      <c r="B35" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C35" t="str">
-        <v/>
-      </c>
-      <c r="D35" t="str">
-        <v/>
-      </c>
-      <c r="E35" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F35">
-        <v>0.71</v>
-      </c>
-      <c r="G35" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H35" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I35" t="str">
-        <v/>
-      </c>
-      <c r="J35" t="str">
-        <v/>
-      </c>
-      <c r="K35" t="str">
-        <v/>
-      </c>
-      <c r="L35" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M35">
-        <v>0.95</v>
-      </c>
-      <c r="N35" t="str">
-        <v>f1d5e413399fae3b96a699a7e86e1cf0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>2025-02-28</v>
-      </c>
-      <c r="B36" t="str">
-        <v>Rendimentos</v>
-      </c>
-      <c r="C36" t="str">
-        <v/>
-      </c>
-      <c r="D36" t="str">
-        <v/>
-      </c>
-      <c r="E36" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F36">
-        <v>0.73</v>
-      </c>
-      <c r="G36" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H36" t="str">
-        <v>Rendimentos/Investimentos</v>
-      </c>
-      <c r="I36" t="str">
-        <v/>
-      </c>
-      <c r="J36" t="str">
-        <v/>
-      </c>
-      <c r="K36" t="str">
-        <v/>
-      </c>
-      <c r="L36" t="str">
-        <v>Palavra-chave 'Rendimentos', classificado como rendimento de investimento</v>
-      </c>
-      <c r="M36">
-        <v>0.95</v>
-      </c>
-      <c r="N36" t="str">
-        <v>c211ab5c2345eb4f3436abb124d5377d</v>
+        <v>68d9fd02-5cc9-4211-a7aa-a3b6443e1017</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N25"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2027,98 +1543,98 @@
         <v>Transferência a terceiros</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>-422.42</v>
+        <v>1363.7</v>
       </c>
       <c r="E2">
-        <v>-52.8</v>
+        <v>151.52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Transporte</v>
+        <v>Renda</v>
       </c>
       <c r="B3" t="str">
-        <v>Combustível/Estacionamento</v>
+        <v>Rendimentos/Investimentos</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>-100</v>
+        <v>8.07</v>
       </c>
       <c r="E3">
-        <v>-50</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Saúde</v>
+        <v>Transporte</v>
       </c>
       <c r="B4" t="str">
-        <v>Farmácia</v>
+        <v>App</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>-24.93</v>
+        <v>-44.59</v>
       </c>
       <c r="E4">
-        <v>-24.93</v>
+        <v>-14.86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Renda</v>
+        <v>Alimentação</v>
       </c>
       <c r="B5" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Restaurante</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>33.61</v>
+        <v>-271.62</v>
       </c>
       <c r="E5">
-        <v>1.68</v>
+        <v>-90.54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Investimentos</v>
+        <v>Educação</v>
       </c>
       <c r="B6" t="str">
-        <v>Aporte</v>
+        <v>Mensalidade</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>-4000</v>
+        <v>-298</v>
       </c>
       <c r="E6">
-        <v>-1333.33</v>
+        <v>-149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Alimentação</v>
+        <v>Serviços financeiros</v>
       </c>
       <c r="B7" t="str">
-        <v>Supermercado</v>
+        <v>Cartão – Pagamento de fatura</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>-8</v>
+        <v>-757.56</v>
       </c>
       <c r="E7">
-        <v>-8</v>
+        <v>-757.56</v>
       </c>
     </row>
   </sheetData>
@@ -2148,13 +1664,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>211.81</v>
+        <v>3256.98</v>
       </c>
       <c r="B2">
-        <v>4733.55</v>
+        <v>3256.98</v>
       </c>
       <c r="C2">
-        <v>-4521.74</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes nos gráficos e filtros + normalização do db
</commit_message>
<xml_diff>
--- a/extrato_classificado.xlsx
+++ b/extrato_classificado.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,1108 +412,1620 @@
         <v>descricao_original</v>
       </c>
       <c r="C1" t="str">
-        <v>estabelecimento</v>
+        <v>valor</v>
       </c>
       <c r="D1" t="str">
+        <v>tipo</v>
+      </c>
+      <c r="E1" t="str">
+        <v>counterparty_normalized</v>
+      </c>
+      <c r="F1" t="str">
         <v>cnpj</v>
       </c>
-      <c r="E1" t="str">
-        <v>tipo</v>
-      </c>
-      <c r="F1" t="str">
-        <v>valor</v>
-      </c>
       <c r="G1" t="str">
-        <v>categoria</v>
+        <v>meio_pagamento</v>
       </c>
       <c r="H1" t="str">
-        <v>subcategoria</v>
+        <v>category_id</v>
       </c>
       <c r="I1" t="str">
-        <v>meio_pagamento</v>
+        <v>subcategory_id</v>
       </c>
       <c r="J1" t="str">
-        <v>banco_origem</v>
+        <v>categoria_label</v>
       </c>
       <c r="K1" t="str">
-        <v>banco_destino</v>
+        <v>subcategoria_label</v>
       </c>
       <c r="L1" t="str">
+        <v>movement_kind</v>
+      </c>
+      <c r="M1" t="str">
+        <v>is_internal_transfer</v>
+      </c>
+      <c r="N1" t="str">
+        <v>is_card_bill_payment</v>
+      </c>
+      <c r="O1" t="str">
+        <v>is_investment_aporte</v>
+      </c>
+      <c r="P1" t="str">
+        <v>is_investment_rendimento</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>is_refund_or_chargeback</v>
+      </c>
+      <c r="R1" t="str">
         <v>observacoes</v>
       </c>
-      <c r="M1" t="str">
+      <c r="S1" t="str">
         <v>confianca_classificacao</v>
       </c>
-      <c r="N1" t="str">
+      <c r="T1" t="str">
         <v>id_transacao</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-09-01</v>
+        <v>2025-08-01</v>
       </c>
       <c r="B2" t="str">
-        <v>Transferência Recebida - Fred Williams de Oliveira Lima Junior - •••.938.792-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 19569491-2</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Fred Williams de Oliveira Lima Junior</v>
+        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+      </c>
+      <c r="C2">
+        <v>-1594</v>
       </c>
       <c r="D2" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E2" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F2">
-        <v>1591.35</v>
+        <v>ARTHUR ANDRADE NUNES</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Transferência a terceiros</v>
+        <v>PIX</v>
+      </c>
+      <c r="H2">
+        <v>701</v>
       </c>
       <c r="I2" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J2" t="str">
-        <v>NU PAGAMENTOS</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K2" t="str">
         <v/>
       </c>
       <c r="L2" t="str">
-        <v>Transferência recebida via PIX, favorecido não parece o titular, classificado como transferência a terceiros.</v>
+        <v>transfer</v>
       </c>
       <c r="M2">
-        <v>0.65</v>
-      </c>
-      <c r="N2" t="str">
-        <v>68b58bc1-95c1-43af-8dd9-6e79ffa7981c</v>
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="str">
+        <v>Destinatário coincide com titular pela regra de transferência interna; flag prioritária ativada.</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="str">
+        <v>688c91f8-c9ef-4d4f-8121-5c8af57ac0f3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-09-01</v>
+        <v>2025-08-02</v>
       </c>
       <c r="B3" t="str">
-        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
       </c>
       <c r="D3" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E3" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F3">
-        <v>1591.35</v>
+        <v>ADISRAELY C ANDRADE SILVA</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
       </c>
       <c r="G3" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H3">
+        <v>700</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
         <v>Transferências</v>
       </c>
-      <c r="H3" t="str">
-        <v>Transferência a terceiros</v>
-      </c>
-      <c r="I3" t="str">
-        <v>PIX</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
       <c r="K3" t="str">
-        <v>MERCADO PAGO IP LTDA.</v>
+        <v/>
       </c>
       <c r="L3" t="str">
-        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
+        <v>transfer</v>
       </c>
       <c r="M3">
-        <v>0.65</v>
-      </c>
-      <c r="N3" t="str">
-        <v>68b59f38-3b11-43af-8ce2-6619375c06fb</v>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="str">
+        <v>Transferência recebida via Pix de terceiro. Sem relação ao titular; padrão de transferência identificado; sem regra pessoal. Renda não habitual.</v>
+      </c>
+      <c r="S3">
+        <v>0.8</v>
+      </c>
+      <c r="T3" t="str">
+        <v>688ea4a4-8930-4d63-b643-f05db7c7286e</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-09-03</v>
+        <v>2025-08-02</v>
       </c>
       <c r="B4" t="str">
-        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Adisraely C Andrade Silva</v>
+        <v>Transferência Recebida - Samir Abfadill Toutenge Neto - •••.978.142-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 26146220-5</v>
+      </c>
+      <c r="C4">
+        <v>23.21</v>
       </c>
       <c r="D4" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E4" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
+        <v>SAMIR ABFADILL TOUTENGE NETO</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
       </c>
       <c r="G4" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H4">
+        <v>700</v>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
         <v>Transferências</v>
       </c>
-      <c r="H4" t="str">
-        <v>Transferência a terceiros</v>
-      </c>
-      <c r="I4" t="str">
-        <v>PIX</v>
-      </c>
-      <c r="J4" t="str">
-        <v>BCO DO BRASIL S.A.</v>
-      </c>
       <c r="K4" t="str">
         <v/>
       </c>
       <c r="L4" t="str">
-        <v>Transferência recebida via PIX de terceiro, não corresponde ao titular.</v>
+        <v>transfer</v>
       </c>
       <c r="M4">
-        <v>0.65</v>
-      </c>
-      <c r="N4" t="str">
-        <v>68b8e7c0-884a-4b9d-ba6a-8769217c588c</v>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem identificação de vínculo pessoal nem regra explícita.</v>
+      </c>
+      <c r="S4">
+        <v>0.8</v>
+      </c>
+      <c r="T4" t="str">
+        <v>688ebe09-6b1d-4972-a0b1-3cc71c89e726</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-09-04</v>
+        <v>2025-08-03</v>
       </c>
       <c r="B5" t="str">
-        <v>Transferência enviada pelo Pix - IGOR VINICIUS GOMES DE OLIVEIRA - •••.869.528-•• - BCO BRADESCO S.A. (0237) Agência: 909 Conta: 3460-6</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Igor Vinicius Gomes de Oliveira</v>
+        <v>Compra no débito - FORT ATACADISTA 810</v>
+      </c>
+      <c r="C5">
+        <v>-167.21</v>
       </c>
       <c r="D5" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E5" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F5">
-        <v>74.25</v>
+        <v>FORT ATACADISTA 810</v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
       </c>
       <c r="G5" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Transferência a terceiros</v>
+        <v>CARTAO_DEBITO</v>
+      </c>
+      <c r="H5">
+        <v>101</v>
       </c>
       <c r="I5" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J5" t="str">
-        <v/>
+        <v>Alimentação/Supermercado</v>
       </c>
       <c r="K5" t="str">
-        <v>BCO BRADESCO S.A.</v>
+        <v/>
       </c>
       <c r="L5" t="str">
-        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
+        <v>spend</v>
       </c>
       <c r="M5">
-        <v>0.65</v>
-      </c>
-      <c r="N5" t="str">
-        <v>68b97efe-de9f-4fde-adc8-550b21ec0f0f</v>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="str">
+        <v>Palavra-chave de supermercados reconhecida em estabelecimento. Nenhuma regra pessoal aplicável.</v>
+      </c>
+      <c r="S5">
+        <v>0.95</v>
+      </c>
+      <c r="T5" t="str">
+        <v>688f64b7-cf2a-4c30-b548-9f94fafa1b83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-09-05</v>
+        <v>2025-08-04</v>
       </c>
       <c r="B6" t="str">
-        <v>Transferência de saldo NuInvest</v>
-      </c>
-      <c r="C6" t="str">
-        <v>NuInvest</v>
+        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
+      </c>
+      <c r="C6">
+        <v>700</v>
       </c>
       <c r="D6" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E6" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F6">
-        <v>1.98</v>
+        <v>ADISRAELY C ANDRADE SILVA</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
       </c>
       <c r="G6" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>PIX</v>
+      </c>
+      <c r="H6">
+        <v>700</v>
       </c>
       <c r="I6" t="str">
-        <v>TEF</v>
+        <v/>
       </c>
       <c r="J6" t="str">
-        <v>NuInvest</v>
+        <v>Transferências</v>
       </c>
       <c r="K6" t="str">
         <v/>
       </c>
       <c r="L6" t="str">
-        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
+        <v>transfer</v>
       </c>
       <c r="M6">
-        <v>0.9</v>
-      </c>
-      <c r="N6" t="str">
-        <v>68bad327-eb76-4d9b-ab6b-8272708e7058</v>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem correspondência a regras pessoais ou salário.</v>
+      </c>
+      <c r="S6">
+        <v>0.8</v>
+      </c>
+      <c r="T6" t="str">
+        <v>68910837-58de-4ab7-9878-336b958f41fd</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-09-06</v>
+        <v>2025-08-05</v>
       </c>
       <c r="B7" t="str">
-        <v>Compra no débito via NuPay - Uber</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Uber</v>
+        <v>Transferência recebida pelo Pix - Arthur Andrade Nunes - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+      </c>
+      <c r="C7">
+        <v>1077.12</v>
       </c>
       <c r="D7" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E7" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F7">
-        <v>21.93</v>
+        <v>ARTHUR ANDRADE NUNES</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
       </c>
       <c r="G7" t="str">
-        <v>Transporte</v>
-      </c>
-      <c r="H7" t="str">
-        <v>App</v>
+        <v>PIX</v>
+      </c>
+      <c r="H7">
+        <v>701</v>
       </c>
       <c r="I7" t="str">
-        <v>cartão débito</v>
+        <v/>
       </c>
       <c r="J7" t="str">
-        <v/>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K7" t="str">
         <v/>
       </c>
       <c r="L7" t="str">
-        <v>Descrição contém 'Uber' (palavra-chave de transporte app).</v>
+        <v>transfer</v>
       </c>
       <c r="M7">
-        <v>0.95</v>
-      </c>
-      <c r="N7" t="str">
-        <v>68bc748b-bb47-48ae-9674-c299fd4451d2</v>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" t="str">
+        <v>Remetente coincide com o titular (transferência interna, alta confiança).</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" t="str">
+        <v>6892751b-25f9-44d8-9ae5-7fcae3c6cae9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-09-11</v>
+        <v>2025-08-05</v>
       </c>
       <c r="B8" t="str">
-        <v>Transferência de saldo NuInvest</v>
-      </c>
-      <c r="C8" t="str">
-        <v>NuInvest</v>
+        <v>Pagamento de fatura</v>
+      </c>
+      <c r="C8">
+        <v>-1121.8</v>
       </c>
       <c r="D8" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E8" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F8">
-        <v>0.09</v>
+        <v>Pagamento de fatura</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
       </c>
       <c r="G8" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H8">
+        <v>502</v>
       </c>
       <c r="I8" t="str">
-        <v>TEF</v>
+        <v/>
       </c>
       <c r="J8" t="str">
-        <v>NuInvest</v>
+        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
       </c>
       <c r="K8" t="str">
         <v/>
       </c>
       <c r="L8" t="str">
-        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
+        <v>transfer</v>
       </c>
       <c r="M8">
-        <v>0.9</v>
-      </c>
-      <c r="N8" t="str">
-        <v>68c2bc51-c9a5-4f97-8310-ec55c7f13e5b</v>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" t="str">
+        <v>Descrição clássica de pagamento de fatura (flag prioritária, não conta como gasto).</v>
+      </c>
+      <c r="S8">
+        <v>0.99</v>
+      </c>
+      <c r="T8" t="str">
+        <v>68927532-f89f-47ce-b36d-3bc180cc13b7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-09-12</v>
+        <v>2025-08-07</v>
       </c>
       <c r="B9" t="str">
         <v>Transferência de saldo NuInvest</v>
       </c>
-      <c r="C9" t="str">
-        <v>NuInvest</v>
+      <c r="C9">
+        <v>1.98</v>
       </c>
       <c r="D9" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E9" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F9">
-        <v>0.82</v>
+        <v>NUINVEST</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
       </c>
       <c r="G9" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H9" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H9">
+        <v>602</v>
       </c>
       <c r="I9" t="str">
-        <v>TEF</v>
+        <v/>
       </c>
       <c r="J9" t="str">
-        <v>NuInvest</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K9" t="str">
         <v/>
       </c>
       <c r="L9" t="str">
-        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
+        <v>income</v>
       </c>
       <c r="M9">
-        <v>0.9</v>
-      </c>
-      <c r="N9" t="str">
-        <v>68c40e37-2615-4d5c-884c-c2b6eb593755</v>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9" t="str">
+        <v>Proveniente de corretora, sugestivo de rendimento de investimento (NuInvest); palavra-chave detectada.</v>
+      </c>
+      <c r="S9">
+        <v>0.95</v>
+      </c>
+      <c r="T9" t="str">
+        <v>6894983b-845a-4783-9318-8e1a9c745dba</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-09-12</v>
+        <v>2025-08-08</v>
       </c>
       <c r="B10" t="str">
-        <v>Transferência de saldo NuInvest</v>
-      </c>
-      <c r="C10" t="str">
-        <v>NuInvest</v>
+        <v>Compra no débito - ADIQPLU*FLORIPA MAIS I</v>
+      </c>
+      <c r="C10">
+        <v>-700</v>
       </c>
       <c r="D10" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E10" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F10">
-        <v>1.2</v>
+        <v>ADIQPLU*FLORIPA MAIS I</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
       </c>
       <c r="G10" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>CARTAO_DEBITO</v>
+      </c>
+      <c r="H10">
+        <v>1401</v>
       </c>
       <c r="I10" t="str">
-        <v>TEF</v>
+        <v/>
       </c>
       <c r="J10" t="str">
-        <v>NuInvest</v>
+        <v>Outros/Diversos</v>
       </c>
       <c r="K10" t="str">
         <v/>
       </c>
       <c r="L10" t="str">
-        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
+        <v>spend</v>
       </c>
       <c r="M10">
-        <v>0.9</v>
-      </c>
-      <c r="N10" t="str">
-        <v>68c40e37-d692-4c74-a8f0-7da6a7004150</v>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10" t="str">
+        <v>Estabelecimento não reconhecido em palavras-chave nem regra pessoal, categorizado em Outros.</v>
+      </c>
+      <c r="S10">
+        <v>0.35</v>
+      </c>
+      <c r="T10" t="str">
+        <v>6895f56f-790f-4501-9a35-6bb4d9449d5e</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-09-12</v>
+        <v>2025-08-11</v>
       </c>
       <c r="B11" t="str">
-        <v>Transferência de saldo NuInvest</v>
-      </c>
-      <c r="C11" t="str">
-        <v>NuInvest</v>
+        <v>Transferência Recebida - Fred Williams de Oliveira Lima Junior - •••.938.792-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 19569491-2</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
       </c>
       <c r="D11" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E11" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F11">
-        <v>0.74</v>
+        <v>FRED WILLIAMS DE OLIVEIRA LIMA JUNIOR</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
       </c>
       <c r="G11" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>PIX</v>
+      </c>
+      <c r="H11">
+        <v>700</v>
       </c>
       <c r="I11" t="str">
-        <v>TEF</v>
+        <v/>
       </c>
       <c r="J11" t="str">
-        <v>NuInvest</v>
+        <v>Transferências</v>
       </c>
       <c r="K11" t="str">
         <v/>
       </c>
       <c r="L11" t="str">
-        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
+        <v>transfer</v>
       </c>
       <c r="M11">
-        <v>0.9</v>
-      </c>
-      <c r="N11" t="str">
-        <v>68c40e38-45e2-44a3-9d29-aba78f835f0d</v>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem regra pessoal ou vínculo identificado.</v>
+      </c>
+      <c r="S11">
+        <v>0.8</v>
+      </c>
+      <c r="T11" t="str">
+        <v>689a550e-466f-465f-8991-74d02b7c2541</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-09-12</v>
+        <v>2025-08-11</v>
       </c>
       <c r="B12" t="str">
-        <v>Transferência de saldo NuInvest</v>
-      </c>
-      <c r="C12" t="str">
-        <v>NuInvest</v>
+        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+      </c>
+      <c r="C12">
+        <v>-50</v>
       </c>
       <c r="D12" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E12" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F12">
-        <v>3.24</v>
+        <v>ARTHUR ANDRADE NUNES</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
       </c>
       <c r="G12" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="H12" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>PIX</v>
+      </c>
+      <c r="H12">
+        <v>701</v>
       </c>
       <c r="I12" t="str">
-        <v>TEF</v>
+        <v/>
       </c>
       <c r="J12" t="str">
-        <v>NuInvest</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K12" t="str">
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>Transferência de saldo proveniente de corretora; geralmente resgate/rendimento.</v>
+        <v>transfer</v>
       </c>
       <c r="M12">
-        <v>0.9</v>
-      </c>
-      <c r="N12" t="str">
-        <v>68c40e3a-fc05-41ec-88b8-b8f30506276c</v>
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12" t="str">
+        <v>Destinatário coincide com titular pela regra de transferência interna.</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12" t="str">
+        <v>689a7122-0ac3-447b-b0bd-c4e810fe3f44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-09-17</v>
+        <v>2025-08-13</v>
       </c>
       <c r="B13" t="str">
-        <v>Compra no débito - MINI KALZONE</v>
-      </c>
-      <c r="C13" t="str">
-        <v>MINI KALZONE</v>
+        <v>Transferência de saldo NuInvest</v>
+      </c>
+      <c r="C13">
+        <v>0.1</v>
       </c>
       <c r="D13" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E13" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
+        <v>NUINVEST</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
       </c>
       <c r="G13" t="str">
-        <v>Alimentação</v>
-      </c>
-      <c r="H13" t="str">
-        <v>Restaurante</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H13">
+        <v>602</v>
       </c>
       <c r="I13" t="str">
-        <v>cartão débito</v>
+        <v/>
       </c>
       <c r="J13" t="str">
-        <v/>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K13" t="str">
         <v/>
       </c>
       <c r="L13" t="str">
-        <v>Estabelecimento sugere restaurante/fast-food.</v>
+        <v>income</v>
       </c>
       <c r="M13">
-        <v>0.92</v>
-      </c>
-      <c r="N13" t="str">
-        <v>68cb0900-49ea-4f71-b890-bf64f7d0a9eb</v>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13" t="str">
+        <v>Transferência de saldo originada de corretora, interpretada como rendimento de investimento.</v>
+      </c>
+      <c r="S13">
+        <v>0.95</v>
+      </c>
+      <c r="T13" t="str">
+        <v>689c8119-52e0-47f2-9288-f7260f7a0b6e</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-09-22</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B14" t="str">
-        <v>Transferência recebida pelo Pix - EURIVAL BATISTA NUNES - •••.965.195-•• - BCO DO BRASIL S.A. (0001) Agência: 5752 Conta: 6897-7</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Eurival Batista Nunes</v>
+        <v>Transferência de saldo NuInvest</v>
+      </c>
+      <c r="C14">
+        <v>3.24</v>
       </c>
       <c r="D14" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E14" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F14">
-        <v>300</v>
+        <v>NUINVEST</v>
+      </c>
+      <c r="F14" t="str">
+        <v/>
       </c>
       <c r="G14" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H14" t="str">
-        <v>Transferência a terceiros</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H14">
+        <v>602</v>
       </c>
       <c r="I14" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J14" t="str">
-        <v>BCO DO BRASIL S.A.</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K14" t="str">
         <v/>
       </c>
       <c r="L14" t="str">
-        <v>Transferência recebida via PIX de terceiro, não corresponde ao titular.</v>
+        <v>income</v>
       </c>
       <c r="M14">
-        <v>0.65</v>
-      </c>
-      <c r="N14" t="str">
-        <v>68d13fcb-b5f5-48f4-ab48-671f3d23d658</v>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" t="str">
+        <v>Transferência de saldo originada de corretora, interpretada como rendimento de investimento.</v>
+      </c>
+      <c r="S14">
+        <v>0.95</v>
+      </c>
+      <c r="T14" t="str">
+        <v>689dd52b-4c36-4eb8-9a6e-3172b1e32c9f</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-09-22</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B15" t="str">
-        <v>Transferência enviada pelo Pix - ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA - 34.075.739/0001-84 - ITAÚ UNIBANCO S.A. (0341) Agência: 459 Conta: 33230-0</v>
-      </c>
-      <c r="C15" t="str">
-        <v>ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA</v>
+        <v>Transferência de saldo NuInvest</v>
+      </c>
+      <c r="C15">
+        <v>0.82</v>
       </c>
       <c r="D15" t="str">
-        <v>34.075.739/0001-84</v>
+        <v>credito</v>
       </c>
       <c r="E15" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F15">
-        <v>149</v>
+        <v>NUINVEST</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
       </c>
       <c r="G15" t="str">
-        <v>Educação</v>
-      </c>
-      <c r="H15" t="str">
-        <v>Mensalidade</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H15">
+        <v>602</v>
       </c>
       <c r="I15" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J15" t="str">
-        <v/>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K15" t="str">
-        <v>ITAÚ UNIBANCO S.A.</v>
+        <v/>
       </c>
       <c r="L15" t="str">
-        <v>Nome e CNPJ correspondem a instituição de ensino. Palavra-chave 'Escola'.</v>
+        <v>income</v>
       </c>
       <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15" t="str">
+        <v>Transferência de saldo originada de corretora, interpretada como rendimento de investimento.</v>
+      </c>
+      <c r="S15">
         <v>0.95</v>
       </c>
-      <c r="N15" t="str">
-        <v>68d14071-2832-47e2-8b42-f2d9ed2b46bb</v>
+      <c r="T15" t="str">
+        <v>689dd52b-db57-4cef-9647-8f0bb51e14e8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2025-09-22</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B16" t="str">
-        <v>Transferência enviada pelo Pix - ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA - 34.075.739/0001-84 - ITAÚ UNIBANCO S.A. (0341) Agência: 459 Conta: 33230-0</v>
-      </c>
-      <c r="C16" t="str">
-        <v>ESCOLA ESTACIO DE EDUCACAO BASICA MARACANA</v>
+        <v>Transferência de saldo NuInvest</v>
+      </c>
+      <c r="C16">
+        <v>1.2</v>
       </c>
       <c r="D16" t="str">
-        <v>34.075.739/0001-84</v>
+        <v>credito</v>
       </c>
       <c r="E16" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F16">
-        <v>149</v>
+        <v>NUINVEST</v>
+      </c>
+      <c r="F16" t="str">
+        <v/>
       </c>
       <c r="G16" t="str">
-        <v>Educação</v>
-      </c>
-      <c r="H16" t="str">
-        <v>Mensalidade</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H16">
+        <v>602</v>
       </c>
       <c r="I16" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J16" t="str">
-        <v/>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K16" t="str">
-        <v>ITAÚ UNIBANCO S.A.</v>
+        <v/>
       </c>
       <c r="L16" t="str">
-        <v>Nome e CNPJ correspondem a instituição de ensino. Palavra-chave 'Escola'. Possível duplicidade de pagamento.</v>
+        <v>income</v>
       </c>
       <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="str">
+        <v>Transferência de saldo originada de corretora, interpretada como rendimento de investimento.</v>
+      </c>
+      <c r="S16">
         <v>0.95</v>
       </c>
-      <c r="N16" t="str">
-        <v>68d17dba-ac23-4282-8808-cd3377be4ab3</v>
+      <c r="T16" t="str">
+        <v>689dd52c-0d3a-4163-a990-a7dba774d498</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2025-09-26</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B17" t="str">
-        <v>Transferência recebida pelo Pix - Arthur Andrade Nunes - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
-      </c>
-      <c r="C17" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Transferência de saldo NuInvest</v>
+      </c>
+      <c r="C17">
+        <v>0.91</v>
       </c>
       <c r="D17" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E17" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F17">
-        <v>757.56</v>
+        <v>NUINVEST</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
       </c>
       <c r="G17" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H17" t="str">
-        <v>Transferência a terceiros</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H17">
+        <v>602</v>
       </c>
       <c r="I17" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J17" t="str">
-        <v>MERCADO PAGO IP LTDA.</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K17" t="str">
         <v/>
       </c>
       <c r="L17" t="str">
-        <v>Transferência recebida via PIX, favorecido não parece o titular, classificado como transferência a terceiros.</v>
+        <v>income</v>
       </c>
       <c r="M17">
-        <v>0.65</v>
-      </c>
-      <c r="N17" t="str">
-        <v>68d713ea-986d-45fe-842d-975fc51a17f0</v>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17" t="str">
+        <v>Transferência de saldo originada de corretora, interpretada como rendimento de investimento.</v>
+      </c>
+      <c r="S17">
+        <v>0.95</v>
+      </c>
+      <c r="T17" t="str">
+        <v>689dd52c-e2df-439c-bddb-9f389ac76640</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2025-09-26</v>
+        <v>2025-08-15</v>
       </c>
       <c r="B18" t="str">
-        <v>Pagamento de fatura</v>
-      </c>
-      <c r="C18" t="str">
-        <v/>
+        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
+      </c>
+      <c r="C18">
+        <v>250</v>
       </c>
       <c r="D18" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E18" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F18">
-        <v>757.56</v>
+        <v>ADISRAELY C ANDRADE SILVA</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
       </c>
       <c r="G18" t="str">
-        <v>Serviços financeiros</v>
-      </c>
-      <c r="H18" t="str">
-        <v>Cartão – Pagamento de fatura</v>
+        <v>PIX</v>
+      </c>
+      <c r="H18">
+        <v>700</v>
       </c>
       <c r="I18" t="str">
-        <v>cartão crédito</v>
+        <v/>
       </c>
       <c r="J18" t="str">
-        <v/>
+        <v>Transferências</v>
       </c>
       <c r="K18" t="str">
         <v/>
       </c>
       <c r="L18" t="str">
-        <v>Pagamento de fatura de cartão, não computar como gasto novo (liquidação). Excluir do total de saídas.</v>
+        <v>transfer</v>
       </c>
       <c r="M18">
-        <v>0.99</v>
-      </c>
-      <c r="N18" t="str">
-        <v>68d713ff-5ac6-4d47-9674-c135d7aeeb31</v>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem vínculo de interna nem regra pessoal.</v>
+      </c>
+      <c r="S18">
+        <v>0.8</v>
+      </c>
+      <c r="T18" t="str">
+        <v>689f2bee-d2d2-4afb-8efb-5ef1f6e96d9c</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2025-09-27</v>
+        <v>2025-08-17</v>
       </c>
       <c r="B19" t="str">
-        <v>Transferência recebida pelo Pix - JOHN LUCAS MAGNAVITA DE ALMEIDA - •••.924.005-•• - BANCO INTER (0077) Agência: 1 Conta: 36925596-8</v>
-      </c>
-      <c r="C19" t="str">
-        <v>John Lucas Magnavita de Almeida</v>
+        <v>Transferência recebida pelo Pix - MARCOS ANTONIO SOUZA FILHO - •••.846.039-•• - CC UNICRED VALOR CAPITAL LTDA - UNICRED VALOR CAPITAL Agência: 1108 Conta: 71941-2</v>
+      </c>
+      <c r="C19">
+        <v>17.18</v>
       </c>
       <c r="D19" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E19" t="str">
-        <v>credito</v>
-      </c>
-      <c r="F19">
-        <v>500</v>
+        <v>MARCOS ANTONIO SOUZA FILHO</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
       </c>
       <c r="G19" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H19">
+        <v>700</v>
+      </c>
+      <c r="I19" t="str">
+        <v/>
+      </c>
+      <c r="J19" t="str">
         <v>Transferências</v>
       </c>
-      <c r="H19" t="str">
-        <v>Transferência a terceiros</v>
-      </c>
-      <c r="I19" t="str">
-        <v>PIX</v>
-      </c>
-      <c r="J19" t="str">
-        <v>BANCO INTER</v>
-      </c>
       <c r="K19" t="str">
         <v/>
       </c>
       <c r="L19" t="str">
-        <v>Transferência recebida via PIX de terceiro, não corresponde ao titular.</v>
+        <v>transfer</v>
       </c>
       <c r="M19">
-        <v>0.65</v>
-      </c>
-      <c r="N19" t="str">
-        <v>68d81c64-7ae7-4337-a9d0-c8ca9268abb1</v>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem vínculo de interna nem regra pessoal.</v>
+      </c>
+      <c r="S19">
+        <v>0.8</v>
+      </c>
+      <c r="T19" t="str">
+        <v>68a1ee13-1695-47ea-8fee-6146d86bea20</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2025-09-27</v>
+        <v>2025-08-18</v>
       </c>
       <c r="B20" t="str">
-        <v>Compra no débito via NuPay - Uber</v>
-      </c>
-      <c r="C20" t="str">
-        <v>Uber</v>
+        <v>Transferência Recebida - Miriã dos Reis Almeida - •••.758.569-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 41331813-8</v>
+      </c>
+      <c r="C20">
+        <v>17.18</v>
       </c>
       <c r="D20" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E20" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F20">
-        <v>13.23</v>
+        <v>MIRIÃ DOS REIS ALMEIDA</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
       </c>
       <c r="G20" t="str">
-        <v>Transporte</v>
-      </c>
-      <c r="H20" t="str">
-        <v>App</v>
+        <v>PIX</v>
+      </c>
+      <c r="H20">
+        <v>700</v>
       </c>
       <c r="I20" t="str">
-        <v>cartão débito</v>
+        <v/>
       </c>
       <c r="J20" t="str">
-        <v/>
+        <v>Transferências</v>
       </c>
       <c r="K20" t="str">
         <v/>
       </c>
       <c r="L20" t="str">
-        <v>Descrição contém 'Uber' (palavra-chave de transporte app).</v>
+        <v>transfer</v>
       </c>
       <c r="M20">
-        <v>0.95</v>
-      </c>
-      <c r="N20" t="str">
-        <v>68d86970-7e36-4f39-9c0b-7c35eb994be3</v>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem correspondência a regras pessoais ou salário.</v>
+      </c>
+      <c r="S20">
+        <v>0.8</v>
+      </c>
+      <c r="T20" t="str">
+        <v>68a39be4-f946-41ec-b037-aa6c2f7e9922</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2025-09-27</v>
+        <v>2025-08-18</v>
       </c>
       <c r="B21" t="str">
-        <v>Compra no débito - JeronimoFlorianop</v>
-      </c>
-      <c r="C21" t="str">
-        <v>JeronimoFlorianop</v>
+        <v>Transferência recebida pelo Pix - JOAO HENRIQUE L S A GUERRA - •••.423.549-•• - ITAÚ UNIBANCO S.A. (0341) Agência: 8560 Conta: 23137-8</v>
+      </c>
+      <c r="C21">
+        <v>17.18</v>
       </c>
       <c r="D21" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E21" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F21">
-        <v>57</v>
+        <v>JOAO HENRIQUE L S A GUERRA</v>
+      </c>
+      <c r="F21" t="str">
+        <v/>
       </c>
       <c r="G21" t="str">
-        <v>Alimentação</v>
-      </c>
-      <c r="H21" t="str">
-        <v>Restaurante</v>
+        <v>PIX</v>
+      </c>
+      <c r="H21">
+        <v>700</v>
       </c>
       <c r="I21" t="str">
-        <v>cartão débito</v>
+        <v/>
       </c>
       <c r="J21" t="str">
-        <v/>
+        <v>Transferências</v>
       </c>
       <c r="K21" t="str">
         <v/>
       </c>
       <c r="L21" t="str">
-        <v>Estabelecimento aparenta ser restaurante de fast food. Pela convenção da marca Jeronimo, classificado como Alimentação/Restaurante.</v>
+        <v>transfer</v>
       </c>
       <c r="M21">
-        <v>0.9</v>
-      </c>
-      <c r="N21" t="str">
-        <v>68d87576-526a-4e24-995d-a214ec00ee05</v>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" t="str">
+        <v>Transferência recebida de terceiro via Pix. Sem correspondência a regras pessoais ou salário.</v>
+      </c>
+      <c r="S21">
+        <v>0.8</v>
+      </c>
+      <c r="T21" t="str">
+        <v>68a3b377-18fb-4309-ba00-f924bd71a7cb</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>2025-09-27</v>
+        <v>2025-08-20</v>
       </c>
       <c r="B22" t="str">
-        <v>Transferência enviada pelo Pix - Miriã dos Reis Almeida - •••.758.569-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 41331813-8</v>
-      </c>
-      <c r="C22" t="str">
-        <v>Miriã dos Reis Almeida</v>
+        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+      </c>
+      <c r="C22">
+        <v>-250</v>
       </c>
       <c r="D22" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E22" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F22">
-        <v>13</v>
+        <v>ARTHUR ANDRADE NUNES</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
       </c>
       <c r="G22" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H22" t="str">
-        <v>Transferência a terceiros</v>
+        <v>PIX</v>
+      </c>
+      <c r="H22">
+        <v>701</v>
       </c>
       <c r="I22" t="str">
-        <v>PIX</v>
+        <v/>
       </c>
       <c r="J22" t="str">
-        <v/>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K22" t="str">
-        <v>NU PAGAMENTOS</v>
+        <v/>
       </c>
       <c r="L22" t="str">
-        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
+        <v>transfer</v>
       </c>
       <c r="M22">
-        <v>0.65</v>
-      </c>
-      <c r="N22" t="str">
-        <v>68d88096-1f88-4ea5-a1d1-6800f7a58635</v>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22" t="str">
+        <v>Destinatário coincide com titular pela regra de transferência interna (alta prioridade).</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22" t="str">
+        <v>68a5fcbe-2ed9-475d-8a0c-1bd4bad926de</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>2025-09-28</v>
+        <v>2025-08-20</v>
       </c>
       <c r="B23" t="str">
         <v>Compra no débito via NuPay - Uber</v>
       </c>
-      <c r="C23" t="str">
-        <v>Uber</v>
+      <c r="C23">
+        <v>-6.86</v>
       </c>
       <c r="D23" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E23" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F23">
-        <v>9.43</v>
+        <v>UBER</v>
+      </c>
+      <c r="F23" t="str">
+        <v/>
       </c>
       <c r="G23" t="str">
-        <v>Transporte</v>
-      </c>
-      <c r="H23" t="str">
-        <v>App</v>
+        <v>CARTAO_DEBITO</v>
+      </c>
+      <c r="H23">
+        <v>202</v>
       </c>
       <c r="I23" t="str">
-        <v>cartão débito</v>
+        <v/>
       </c>
       <c r="J23" t="str">
-        <v/>
+        <v>Transporte/App</v>
       </c>
       <c r="K23" t="str">
         <v/>
       </c>
       <c r="L23" t="str">
-        <v>Descrição contém 'Uber' (palavra-chave de transporte app).</v>
+        <v>spend</v>
       </c>
       <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23" t="str">
+        <v>Palavra-chave clássica de transporte por aplicativo (Uber) detectada.</v>
+      </c>
+      <c r="S23">
         <v>0.95</v>
       </c>
-      <c r="N23" t="str">
-        <v>68d9c2ae-9c68-4cde-aa22-740d26f291d6</v>
+      <c r="T23" t="str">
+        <v>68a642d1-fead-48b9-aebf-c5f97d7d5e3c</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>2025-09-28</v>
+        <v>2025-08-26</v>
       </c>
       <c r="B24" t="str">
-        <v>Compra no débito - OUTBACK STEAKHOUSE</v>
-      </c>
-      <c r="C24" t="str">
-        <v>OUTBACK STEAKHOUSE</v>
+        <v>Pagamento de fatura</v>
+      </c>
+      <c r="C24">
+        <v>-52.93</v>
       </c>
       <c r="D24" t="str">
-        <v/>
+        <v>debito</v>
       </c>
       <c r="E24" t="str">
-        <v>debito</v>
-      </c>
-      <c r="F24">
-        <v>204.62</v>
+        <v>Pagamento de fatura</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
       </c>
       <c r="G24" t="str">
-        <v>Alimentação</v>
-      </c>
-      <c r="H24" t="str">
-        <v>Restaurante</v>
+        <v>OUTRO</v>
+      </c>
+      <c r="H24">
+        <v>502</v>
       </c>
       <c r="I24" t="str">
-        <v>cartão débito</v>
+        <v/>
       </c>
       <c r="J24" t="str">
-        <v/>
+        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
       </c>
       <c r="K24" t="str">
         <v/>
       </c>
       <c r="L24" t="str">
-        <v>Nome do estabelecimento é de restaurante, classificado como Alimentação/Restaurante.</v>
+        <v>transfer</v>
       </c>
       <c r="M24">
-        <v>0.98</v>
-      </c>
-      <c r="N24" t="str">
-        <v>68d9dbad-042c-46d0-aec6-430cf5ffef54</v>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24" t="str">
+        <v>Descrição clássica de pagamento de fatura. Flag ativada.</v>
+      </c>
+      <c r="S24">
+        <v>0.99</v>
+      </c>
+      <c r="T24" t="str">
+        <v>68ae3f06-b81e-458e-ad35-f49e5acfa734</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>2025-09-29</v>
+        <v>2025-08-26</v>
       </c>
       <c r="B25" t="str">
-        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
-      </c>
-      <c r="C25" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Transferência recebida pelo Pix - Arthur Andrade Nunes - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+      </c>
+      <c r="C25">
+        <v>586.7</v>
       </c>
       <c r="D25" t="str">
-        <v/>
+        <v>credito</v>
       </c>
       <c r="E25" t="str">
+        <v>ARTHUR ANDRADE NUNES</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+      <c r="G25" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H25">
+        <v>701</v>
+      </c>
+      <c r="I25" t="str">
+        <v/>
+      </c>
+      <c r="J25" t="str">
+        <v>Transferências/Interna (Movimentação bancária)</v>
+      </c>
+      <c r="K25" t="str">
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <v>transfer</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25" t="str">
+        <v>Remetente coincide com titular (transferência interna).</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25" t="str">
+        <v>68ae3f59-d9a8-4285-bd89-4f33c70466c6</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>2025-08-26</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Pagamento de fatura</v>
+      </c>
+      <c r="C26">
+        <v>-586.7</v>
+      </c>
+      <c r="D26" t="str">
         <v>debito</v>
       </c>
-      <c r="F25">
-        <v>206.61</v>
-      </c>
-      <c r="G25" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="H25" t="str">
-        <v>Transferência a terceiros</v>
-      </c>
-      <c r="I25" t="str">
-        <v>PIX</v>
-      </c>
-      <c r="J25" t="str">
-        <v/>
-      </c>
-      <c r="K25" t="str">
-        <v>MERCADO PAGO IP LTDA.</v>
-      </c>
-      <c r="L25" t="str">
-        <v>Transferência enviada via PIX para terceiro, não corresponde ao titular.</v>
-      </c>
-      <c r="M25">
-        <v>0.65</v>
-      </c>
-      <c r="N25" t="str">
-        <v>68d9fd02-5cc9-4211-a7aa-a3b6443e1017</v>
+      <c r="E26" t="str">
+        <v>Pagamento de fatura</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H26">
+        <v>502</v>
+      </c>
+      <c r="I26" t="str">
+        <v/>
+      </c>
+      <c r="J26" t="str">
+        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+      </c>
+      <c r="K26" t="str">
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <v>transfer</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26" t="str">
+        <v>Descrição clássica de pagamento de fatura. Flag ativada.</v>
+      </c>
+      <c r="S26">
+        <v>0.99</v>
+      </c>
+      <c r="T26" t="str">
+        <v>68ae3f6c-7880-44ba-a47d-d3be1da21b3d</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T26"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1537,109 +2049,105 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Transferências</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Transferência a terceiros</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1363.7</v>
+        <v>-230.18</v>
       </c>
       <c r="E2">
-        <v>151.52</v>
+        <v>-46.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Renda</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Rendimentos/Investimentos</v>
+        <v>Transferências</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>8.07</v>
+        <v>1174.75</v>
       </c>
       <c r="E3">
-        <v>1.34</v>
+        <v>146.84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Transporte</v>
-      </c>
-      <c r="B4" t="str">
-        <v>App</v>
+        <v>Alimentação/Supermercado</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>-44.59</v>
+        <v>-167.21</v>
       </c>
       <c r="E4">
-        <v>-14.86</v>
+        <v>-167.21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Alimentação</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Restaurante</v>
+        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>-271.62</v>
+        <v>-1761.43</v>
       </c>
       <c r="E5">
-        <v>-90.54</v>
+        <v>-587.14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Educação</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Mensalidade</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>-298</v>
+        <v>8.25</v>
       </c>
       <c r="E6">
-        <v>-149</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Serviços financeiros</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Cartão – Pagamento de fatura</v>
+        <v>Outros/Diversos</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>-757.56</v>
+        <v>-700</v>
       </c>
       <c r="E7">
-        <v>-757.56</v>
+        <v>-700</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Transporte/App</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>-6.86</v>
+      </c>
+      <c r="E8">
+        <v>-6.86</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1664,13 +2172,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3256.98</v>
+        <v>2846.82</v>
       </c>
       <c r="B2">
-        <v>3256.98</v>
+        <v>874.07</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1972.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
migração do banco para postgres
</commit_message>
<xml_diff>
--- a/extrato_classificado.xlsx
+++ b/extrato_classificado.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -471,40 +471,40 @@
         <v>2025-08-01</v>
       </c>
       <c r="B2" t="str">
-        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C2">
-        <v>-1594</v>
+        <v>0.02</v>
       </c>
       <c r="D2" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E2" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F2" t="str">
         <v/>
       </c>
       <c r="G2" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H2">
-        <v>701</v>
-      </c>
-      <c r="I2">
-        <v>701</v>
+        <v>602</v>
+      </c>
+      <c r="I2" t="str">
+        <v/>
       </c>
       <c r="J2" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K2" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v/>
       </c>
       <c r="L2" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -513,36 +513,36 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="str">
-        <v>Prioridade 1: detectada transferência interna por nome do titular (Arthur Andrade Nunes). Não contabilizado como gasto.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="T2" t="str">
-        <v>688c91f8-c9ef-4d4f-8121-5c8af57ac0f3</v>
+        <v>1732036091847</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-01</v>
       </c>
       <c r="B3" t="str">
-        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
+        <v>Transferência Pix recebida Wise Brasil Corretora de CÃ¢mbio Ltda.</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>439.98</v>
       </c>
       <c r="D3" t="str">
         <v>credito</v>
       </c>
       <c r="E3" t="str">
-        <v>Adisraely C Andrade Silva</v>
+        <v>Wise Brasil Corretora de Câmbio Ltda.</v>
       </c>
       <c r="F3" t="str">
         <v/>
@@ -551,19 +551,19 @@
         <v>PIX</v>
       </c>
       <c r="H3">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I3" t="str">
         <v/>
       </c>
       <c r="J3" t="str">
-        <v>Transferências</v>
+        <v>Renda/Salário</v>
       </c>
       <c r="K3" t="str">
         <v/>
       </c>
       <c r="L3" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -581,30 +581,30 @@
         <v>0</v>
       </c>
       <c r="R3" t="str">
-        <v>Transferência recebida via PIX de terceiro. Sem relação explícita com titular.</v>
+        <v>Regra do usuário: Wise Brasil Corretora de Câmbio Ltda. = salário.</v>
       </c>
       <c r="S3">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="T3" t="str">
-        <v>688ea4a4-8930-4d63-b643-f05db7c7286e</v>
+        <v>120601361492</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-01</v>
       </c>
       <c r="B4" t="str">
-        <v>Transferência Recebida - Samir Abfadill Toutenge Neto - •••.978.142-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 26146220-5</v>
+        <v>Transferência Pix recebida Arthur Andrade Nunes</v>
       </c>
       <c r="C4">
-        <v>23.21</v>
+        <v>1594</v>
       </c>
       <c r="D4" t="str">
         <v>credito</v>
       </c>
       <c r="E4" t="str">
-        <v>Samir Abfadill Toutenge Neto</v>
+        <v>Arthur Andrade Nunes</v>
       </c>
       <c r="F4" t="str">
         <v/>
@@ -613,13 +613,13 @@
         <v>PIX</v>
       </c>
       <c r="H4">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="I4" t="str">
         <v/>
       </c>
       <c r="J4" t="str">
-        <v>Transferências</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K4" t="str">
         <v/>
@@ -628,7 +628,7 @@
         <v>transfer</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -643,45 +643,45 @@
         <v>0</v>
       </c>
       <c r="R4" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Transferência recebida do próprio titular; detectada transferência interna.</v>
       </c>
       <c r="S4">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="T4" t="str">
-        <v>688ebe09-6b1d-4972-a0b1-3cc71c89e726</v>
+        <v>120084774783</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-08-03</v>
+        <v>2025-08-01</v>
       </c>
       <c r="B5" t="str">
-        <v>Compra no débito - FORT ATACADISTA 810</v>
+        <v>Pagamento de contas Banco Cooperativo Sicredi S. A.</v>
       </c>
       <c r="C5">
-        <v>-167.21</v>
+        <v>-809.03</v>
       </c>
       <c r="D5" t="str">
         <v>debito</v>
       </c>
       <c r="E5" t="str">
-        <v>Fort Atacadista 810</v>
+        <v>Banco Cooperativo Sicredi S. A.</v>
       </c>
       <c r="F5" t="str">
         <v/>
       </c>
       <c r="G5" t="str">
-        <v>CARTAO_DEBITO</v>
+        <v>OUTRO</v>
       </c>
       <c r="H5">
-        <v>101</v>
+        <v>810</v>
       </c>
       <c r="I5" t="str">
         <v/>
       </c>
       <c r="J5" t="str">
-        <v>Alimentação/Supermercado</v>
+        <v>Moradia/Condomínio</v>
       </c>
       <c r="K5" t="str">
         <v/>
@@ -705,13 +705,13 @@
         <v>0</v>
       </c>
       <c r="R5" t="str">
-        <v>Palavra-chave 'ATACAD' reconhecida (supermercado).</v>
+        <v>Regra do usuário para Banco Cooperativo Sicredi S. A.</v>
       </c>
       <c r="S5">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="T5" t="str">
-        <v>688f64b7-cf2a-4c30-b548-9f94fafa1b83</v>
+        <v>120084723379</v>
       </c>
     </row>
     <row r="6">
@@ -719,37 +719,37 @@
         <v>2025-08-04</v>
       </c>
       <c r="B6" t="str">
-        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C6">
-        <v>700</v>
+        <v>0.57</v>
       </c>
       <c r="D6" t="str">
         <v>credito</v>
       </c>
       <c r="E6" t="str">
-        <v>Adisraely C Andrade Silva</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F6" t="str">
         <v/>
       </c>
       <c r="G6" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H6">
-        <v>700</v>
+        <v>602</v>
       </c>
       <c r="I6" t="str">
         <v/>
       </c>
       <c r="J6" t="str">
-        <v>Transferências</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K6" t="str">
         <v/>
       </c>
       <c r="L6" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -761,19 +761,19 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S6">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="T6" t="str">
-        <v>68910837-58de-4ab7-9878-336b958f41fd</v>
+        <v>1732089964368</v>
       </c>
     </row>
     <row r="7">
@@ -781,40 +781,40 @@
         <v>2025-08-05</v>
       </c>
       <c r="B7" t="str">
-        <v>Transferência recebida pelo Pix - Arthur Andrade Nunes - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C7">
-        <v>1077.12</v>
+        <v>0.57</v>
       </c>
       <c r="D7" t="str">
         <v>credito</v>
       </c>
       <c r="E7" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F7" t="str">
         <v/>
       </c>
       <c r="G7" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H7">
-        <v>701</v>
-      </c>
-      <c r="I7">
-        <v>701</v>
+        <v>602</v>
+      </c>
+      <c r="I7" t="str">
+        <v/>
       </c>
       <c r="J7" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K7" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v/>
       </c>
       <c r="L7" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -823,19 +823,19 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="str">
-        <v>Prioridade 1: transferência interna identificada via nome titular.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="T7" t="str">
-        <v>6892751b-25f9-44d8-9ae5-7fcae3c6cae9</v>
+        <v>1732155201341</v>
       </c>
     </row>
     <row r="8">
@@ -843,43 +843,43 @@
         <v>2025-08-05</v>
       </c>
       <c r="B8" t="str">
-        <v>Pagamento de fatura</v>
+        <v>Transferência Pix recebida Wise Brasil Corretora de CÃ¢mbio Ltda.</v>
       </c>
       <c r="C8">
-        <v>-1121.8</v>
+        <v>2708.76</v>
       </c>
       <c r="D8" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E8" t="str">
-        <v>Pagamento de fatura</v>
+        <v>Wise Brasil Corretora de Câmbio Ltda.</v>
       </c>
       <c r="F8" t="str">
         <v/>
       </c>
       <c r="G8" t="str">
-        <v>OUTRO</v>
+        <v>PIX</v>
       </c>
       <c r="H8">
-        <v>502</v>
-      </c>
-      <c r="I8">
-        <v>502</v>
+        <v>800</v>
+      </c>
+      <c r="I8" t="str">
+        <v/>
       </c>
       <c r="J8" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v>Renda/Salário</v>
       </c>
       <c r="K8" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v/>
       </c>
       <c r="L8" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -891,30 +891,30 @@
         <v>0</v>
       </c>
       <c r="R8" t="str">
-        <v>Prioridade 2: pagamento de fatura identificado. Não é gasto.</v>
+        <v>Regra do usuário: Wise Brasil Corretora de Câmbio Ltda. = salário.</v>
       </c>
       <c r="S8">
         <v>1</v>
       </c>
       <c r="T8" t="str">
-        <v>68927532-f89f-47ce-b36d-3bc180cc13b7</v>
+        <v>120620648907</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-08-07</v>
+        <v>2025-08-05</v>
       </c>
       <c r="B9" t="str">
-        <v>Transferência de saldo NuInvest</v>
+        <v>Pagamento de contas Banco Cooperativo do Brasil S/A - Bancoob</v>
       </c>
       <c r="C9">
-        <v>1.98</v>
+        <v>-2378.2</v>
       </c>
       <c r="D9" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E9" t="str">
-        <v>NuInvest</v>
+        <v>Banco Cooperativo do Brasil S/A - Bancoob</v>
       </c>
       <c r="F9" t="str">
         <v/>
@@ -923,19 +923,19 @@
         <v>OUTRO</v>
       </c>
       <c r="H9">
-        <v>602</v>
-      </c>
-      <c r="I9">
-        <v>602</v>
+        <v>811</v>
+      </c>
+      <c r="I9" t="str">
+        <v/>
       </c>
       <c r="J9" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v>Moradia/Aluguel</v>
       </c>
       <c r="K9" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v/>
       </c>
       <c r="L9" t="str">
-        <v>income</v>
+        <v>spend</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -947,60 +947,60 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="str">
-        <v>Rendimento/resgate de investimento detectado por NuInvest + valor positivo.</v>
+        <v>Regra do usuário para Banco Cooperativo do Brasil S/A - Bancoob.</v>
       </c>
       <c r="S9">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="T9" t="str">
-        <v>6894983b-845a-4783-9318-8e1a9c745dba</v>
+        <v>120621051159</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-08-08</v>
+        <v>2025-08-05</v>
       </c>
       <c r="B10" t="str">
-        <v>Compra no débito - ADIQPLU*FLORIPA MAIS I</v>
+        <v>Transferência Pix enviada Arthur Andrade Nunes</v>
       </c>
       <c r="C10">
-        <v>-700</v>
+        <v>-1077.12</v>
       </c>
       <c r="D10" t="str">
         <v>debito</v>
       </c>
       <c r="E10" t="str">
-        <v>Adiqplu Floripa Mais I</v>
+        <v>Arthur Andrade Nunes</v>
       </c>
       <c r="F10" t="str">
         <v/>
       </c>
       <c r="G10" t="str">
-        <v>CARTAO_DEBITO</v>
+        <v>PIX</v>
       </c>
       <c r="H10">
-        <v>1401</v>
-      </c>
-      <c r="I10">
-        <v>1401</v>
+        <v>701</v>
+      </c>
+      <c r="I10" t="str">
+        <v/>
       </c>
       <c r="J10" t="str">
-        <v>Outros/Diversos</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K10" t="str">
-        <v>Outros/Diversos</v>
+        <v/>
       </c>
       <c r="L10" t="str">
-        <v>spend</v>
+        <v>transfer</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1015,30 +1015,30 @@
         <v>0</v>
       </c>
       <c r="R10" t="str">
-        <v>Não há match claro de categoria, descritor genérico. Classificado como Outros/Diversos.</v>
+        <v>Transferência enviada para titular (Arthur Andrade Nunes) — transferência interna.</v>
       </c>
       <c r="S10">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="T10" t="str">
-        <v>6895f56f-790f-4501-9a35-6bb4d9449d5e</v>
+        <v>121139707012</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-08-11</v>
+        <v>2025-08-05</v>
       </c>
       <c r="B11" t="str">
-        <v>Transferência Recebida - Fred Williams de Oliveira Lima Junior - •••.938.792-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 19569491-2</v>
+        <v>Pagamento com QR Pix PERNAMBUCANAS</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>-140.19</v>
       </c>
       <c r="D11" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E11" t="str">
-        <v>Fred Williams de Oliveira Lima Junior</v>
+        <v>Pernambucanas</v>
       </c>
       <c r="F11" t="str">
         <v/>
@@ -1047,19 +1047,19 @@
         <v>PIX</v>
       </c>
       <c r="H11">
-        <v>700</v>
-      </c>
-      <c r="I11" t="str">
-        <v/>
+        <v>1400</v>
+      </c>
+      <c r="I11">
+        <v>1401</v>
       </c>
       <c r="J11" t="str">
-        <v>Transferências</v>
+        <v>Outros</v>
       </c>
       <c r="K11" t="str">
-        <v/>
+        <v>Outros/Diversos</v>
       </c>
       <c r="L11" t="str">
-        <v>transfer</v>
+        <v>spend</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1077,54 +1077,54 @@
         <v>0</v>
       </c>
       <c r="R11" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Pagamento Pix para Pernambucanas. Não há subcategoria específica no catálogo, classificado como Outros/Diversos.</v>
       </c>
       <c r="S11">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="T11" t="str">
-        <v>689a550e-466f-465f-8991-74d02b7c2541</v>
+        <v>121140351298</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-08-11</v>
+        <v>2025-08-06</v>
       </c>
       <c r="B12" t="str">
-        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C12">
-        <v>-50</v>
+        <v>0.57</v>
       </c>
       <c r="D12" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E12" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F12" t="str">
         <v/>
       </c>
       <c r="G12" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H12">
-        <v>701</v>
-      </c>
-      <c r="I12">
-        <v>701</v>
+        <v>602</v>
+      </c>
+      <c r="I12" t="str">
+        <v/>
       </c>
       <c r="J12" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K12" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v/>
       </c>
       <c r="L12" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1133,36 +1133,36 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12" t="str">
-        <v>Prioridade 1: transferência interna identificada via nome de titular.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="T12" t="str">
-        <v>689a7122-0ac3-447b-b0bd-c4e810fe3f44</v>
+        <v>1732207627096</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-08-13</v>
+        <v>2025-08-07</v>
       </c>
       <c r="B13" t="str">
-        <v>Transferência de saldo NuInvest</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="D13" t="str">
         <v>credito</v>
       </c>
       <c r="E13" t="str">
-        <v>NuInvest</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F13" t="str">
         <v/>
@@ -1173,14 +1173,14 @@
       <c r="H13">
         <v>602</v>
       </c>
-      <c r="I13">
-        <v>602</v>
+      <c r="I13" t="str">
+        <v/>
       </c>
       <c r="J13" t="str">
         <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K13" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v/>
       </c>
       <c r="L13" t="str">
         <v>income</v>
@@ -1201,51 +1201,51 @@
         <v>0</v>
       </c>
       <c r="R13" t="str">
-        <v>Rendimento de investimento detectado.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S13">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="T13" t="str">
-        <v>689c8119-52e0-47f2-9288-f7260f7a0b6e</v>
+        <v>1732258880861</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-08-14</v>
+        <v>2025-08-07</v>
       </c>
       <c r="B14" t="str">
-        <v>Transferência de saldo NuInvest</v>
+        <v>Pagamento com QR Pix CONSORCIO FENIX</v>
       </c>
       <c r="C14">
-        <v>3.24</v>
+        <v>-30</v>
       </c>
       <c r="D14" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E14" t="str">
-        <v>NuInvest</v>
+        <v>CONSORCIO FENIX</v>
       </c>
       <c r="F14" t="str">
         <v/>
       </c>
       <c r="G14" t="str">
-        <v>OUTRO</v>
+        <v>PIX</v>
       </c>
       <c r="H14">
-        <v>602</v>
+        <v>200</v>
       </c>
       <c r="I14">
-        <v>602</v>
+        <v>203</v>
       </c>
       <c r="J14" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v>Transporte</v>
       </c>
       <c r="K14" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v>Transporte/Onibus</v>
       </c>
       <c r="L14" t="str">
-        <v>income</v>
+        <v>spend</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1257,57 +1257,57 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="str">
-        <v>Rendimento de investimento detectado.</v>
+        <v>Regra do usuário: pagamento de ônibus (Consorcio Fenix).</v>
       </c>
       <c r="S14">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="T14" t="str">
-        <v>689dd52b-4c36-4eb8-9a6e-3172b1e32c9f</v>
+        <v>121344312664</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-08-14</v>
+        <v>2025-08-07</v>
       </c>
       <c r="B15" t="str">
-        <v>Transferência de saldo NuInvest</v>
+        <v>Transferência Pix enviada Fred Williams de Oliveira Lima Junior</v>
       </c>
       <c r="C15">
-        <v>0.82</v>
+        <v>-80</v>
       </c>
       <c r="D15" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E15" t="str">
-        <v>NuInvest</v>
+        <v>Fred Williams de Oliveira Lima Junior</v>
       </c>
       <c r="F15" t="str">
         <v/>
       </c>
       <c r="G15" t="str">
-        <v>OUTRO</v>
+        <v>PIX</v>
       </c>
       <c r="H15">
-        <v>602</v>
-      </c>
-      <c r="I15">
-        <v>602</v>
+        <v>700</v>
+      </c>
+      <c r="I15" t="str">
+        <v/>
       </c>
       <c r="J15" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v>Transferências</v>
       </c>
       <c r="K15" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v/>
       </c>
       <c r="L15" t="str">
-        <v>income</v>
+        <v>transfer</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1319,36 +1319,36 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="str">
-        <v>Rendimento de investimento detectado.</v>
+        <v>Transferência Pix enviada para terceiro não identificado como titular.</v>
       </c>
       <c r="S15">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="T15" t="str">
-        <v>689dd52b-db57-4cef-9647-8f0bb51e14e8</v>
+        <v>120892178151</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2025-08-14</v>
+        <v>2025-08-08</v>
       </c>
       <c r="B16" t="str">
-        <v>Transferência de saldo NuInvest</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C16">
-        <v>1.2</v>
+        <v>0.12</v>
       </c>
       <c r="D16" t="str">
         <v>credito</v>
       </c>
       <c r="E16" t="str">
-        <v>NuInvest</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F16" t="str">
         <v/>
@@ -1359,14 +1359,14 @@
       <c r="H16">
         <v>602</v>
       </c>
-      <c r="I16">
-        <v>602</v>
+      <c r="I16" t="str">
+        <v/>
       </c>
       <c r="J16" t="str">
         <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K16" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v/>
       </c>
       <c r="L16" t="str">
         <v>income</v>
@@ -1387,51 +1387,51 @@
         <v>0</v>
       </c>
       <c r="R16" t="str">
-        <v>Rendimento de investimento detectado.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S16">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="T16" t="str">
-        <v>689dd52c-0d3a-4163-a990-a7dba774d498</v>
+        <v>1732315308316</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>2025-08-14</v>
+        <v>2025-08-08</v>
       </c>
       <c r="B17" t="str">
-        <v>Transferência de saldo NuInvest</v>
+        <v>Transferência Pix enviada LUIS ALBERTO SANCHEZ ROJAS</v>
       </c>
       <c r="C17">
-        <v>0.91</v>
+        <v>-130</v>
       </c>
       <c r="D17" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E17" t="str">
-        <v>NuInvest</v>
+        <v>LUIS ALBERTO SANCHEZ ROJAS</v>
       </c>
       <c r="F17" t="str">
         <v/>
       </c>
       <c r="G17" t="str">
-        <v>OUTRO</v>
+        <v>PIX</v>
       </c>
       <c r="H17">
-        <v>602</v>
-      </c>
-      <c r="I17">
-        <v>602</v>
+        <v>700</v>
+      </c>
+      <c r="I17" t="str">
+        <v/>
       </c>
       <c r="J17" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v>Transferências</v>
       </c>
       <c r="K17" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v/>
       </c>
       <c r="L17" t="str">
-        <v>income</v>
+        <v>transfer</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1443,57 +1443,57 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="str">
-        <v>Rendimento de investimento detectado.</v>
+        <v>Transferência Pix para terceiro não em lista de titular.</v>
       </c>
       <c r="S17">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="T17" t="str">
-        <v>689dd52c-e2df-439c-bddb-9f389ac76640</v>
+        <v>121031778185</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>2025-08-15</v>
+        <v>2025-08-11</v>
       </c>
       <c r="B18" t="str">
-        <v>Transferência recebida pelo Pix - ADISRAELY C ANDRADE SILVA - •••.091.122-•• - BCO DO BRASIL S.A. (0001) Agência: 8697 Conta: 9979-1</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C18">
-        <v>250</v>
+        <v>0.07</v>
       </c>
       <c r="D18" t="str">
         <v>credito</v>
       </c>
       <c r="E18" t="str">
-        <v>Adisraely C Andrade Silva</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F18" t="str">
         <v/>
       </c>
       <c r="G18" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H18">
-        <v>700</v>
+        <v>602</v>
       </c>
       <c r="I18" t="str">
         <v/>
       </c>
       <c r="J18" t="str">
-        <v>Transferências</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K18" t="str">
         <v/>
       </c>
       <c r="L18" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1505,36 +1505,36 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S18">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="T18" t="str">
-        <v>689f2bee-d2d2-4afb-8efb-5ef1f6e96d9c</v>
+        <v>1732367562436</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>2025-08-17</v>
+        <v>2025-08-11</v>
       </c>
       <c r="B19" t="str">
-        <v>Transferência recebida pelo Pix - MARCOS ANTONIO SOUZA FILHO - •••.846.039-•• - CC UNICRED VALOR CAPITAL LTDA - UNICRED VALOR CAPITAL Agência: 1108 Conta: 71941-2</v>
+        <v>Transferência Pix recebida Arthur Andrade Nunes</v>
       </c>
       <c r="C19">
-        <v>17.18</v>
+        <v>50</v>
       </c>
       <c r="D19" t="str">
         <v>credito</v>
       </c>
       <c r="E19" t="str">
-        <v>Marcos Antonio Souza Filho</v>
+        <v>Arthur Andrade Nunes</v>
       </c>
       <c r="F19" t="str">
         <v/>
@@ -1543,13 +1543,13 @@
         <v>PIX</v>
       </c>
       <c r="H19">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="I19" t="str">
         <v/>
       </c>
       <c r="J19" t="str">
-        <v>Transferências</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="K19" t="str">
         <v/>
@@ -1558,7 +1558,7 @@
         <v>transfer</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -1573,51 +1573,51 @@
         <v>0</v>
       </c>
       <c r="R19" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Transferência recebida do titular; transferência interna.</v>
       </c>
       <c r="S19">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="T19" t="str">
-        <v>68a1ee13-1695-47ea-8fee-6146d86bea20</v>
+        <v>121922014228</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>2025-08-18</v>
+        <v>2025-08-11</v>
       </c>
       <c r="B20" t="str">
-        <v>Transferência Recebida - Miriã dos Reis Almeida - •••.758.569-•• - NU PAGAMENTOS - IP (0260) Agência: 1 Conta: 41331813-8</v>
+        <v>Pagamento de contas Banco Bradesco S.A.</v>
       </c>
       <c r="C20">
-        <v>17.18</v>
+        <v>-140.57</v>
       </c>
       <c r="D20" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E20" t="str">
-        <v>Miriã dos Reis Almeida</v>
+        <v>Banco Bradesco S.A.</v>
       </c>
       <c r="F20" t="str">
         <v/>
       </c>
       <c r="G20" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H20">
-        <v>700</v>
-      </c>
-      <c r="I20" t="str">
-        <v/>
+        <v>1400</v>
+      </c>
+      <c r="I20">
+        <v>1401</v>
       </c>
       <c r="J20" t="str">
-        <v>Transferências</v>
+        <v>Outros</v>
       </c>
       <c r="K20" t="str">
-        <v/>
+        <v>Outros/Diversos</v>
       </c>
       <c r="L20" t="str">
-        <v>transfer</v>
+        <v>spend</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -1635,51 +1635,51 @@
         <v>0</v>
       </c>
       <c r="R20" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Pagamento de contas (Banco Bradesco) não encaixa em regra de condomínio/aluguel; classificado como Outros.</v>
       </c>
       <c r="S20">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
       <c r="T20" t="str">
-        <v>68a39be4-f946-41ec-b037-aa6c2f7e9922</v>
+        <v>121922138684</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>2025-08-18</v>
+        <v>2025-08-12</v>
       </c>
       <c r="B21" t="str">
-        <v>Transferência recebida pelo Pix - JOAO HENRIQUE L S A GUERRA - •••.423.549-•• - ITAÚ UNIBANCO S.A. (0341) Agência: 8560 Conta: 23137-8</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C21">
-        <v>17.18</v>
+        <v>0.07</v>
       </c>
       <c r="D21" t="str">
         <v>credito</v>
       </c>
       <c r="E21" t="str">
-        <v>Joao Henrique L S A Guerra</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F21" t="str">
         <v/>
       </c>
       <c r="G21" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H21">
-        <v>700</v>
+        <v>602</v>
       </c>
       <c r="I21" t="str">
         <v/>
       </c>
       <c r="J21" t="str">
-        <v>Transferências</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K21" t="str">
         <v/>
       </c>
       <c r="L21" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -1691,60 +1691,60 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
         <v>0</v>
       </c>
       <c r="R21" t="str">
-        <v>Transferência recebida via PIX de terceiro.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S21">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="T21" t="str">
-        <v>68a3b377-18fb-4309-ba00-f924bd71a7cb</v>
+        <v>1732434030684</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>2025-08-20</v>
+        <v>2025-08-13</v>
       </c>
       <c r="B22" t="str">
-        <v>Transferência enviada pelo Pix - ARTHUR ANDRADE NUNES - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C22">
-        <v>-250</v>
+        <v>0.03</v>
       </c>
       <c r="D22" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E22" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F22" t="str">
         <v/>
       </c>
       <c r="G22" t="str">
-        <v>PIX</v>
+        <v>OUTRO</v>
       </c>
       <c r="H22">
-        <v>701</v>
-      </c>
-      <c r="I22">
-        <v>701</v>
+        <v>602</v>
+      </c>
+      <c r="I22" t="str">
+        <v/>
       </c>
       <c r="J22" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K22" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v/>
       </c>
       <c r="L22" t="str">
-        <v>transfer</v>
+        <v>income</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -1753,57 +1753,57 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22">
         <v>0</v>
       </c>
       <c r="R22" t="str">
-        <v>Prioridade 1: transferência interna detectada via nome do titular.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="T22" t="str">
-        <v>68a5fcbe-2ed9-475d-8a0c-1bd4bad926de</v>
+        <v>1732490273616</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>2025-08-20</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B23" t="str">
-        <v>Compra no débito via NuPay - Uber</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C23">
-        <v>-6.86</v>
+        <v>0.03</v>
       </c>
       <c r="D23" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E23" t="str">
-        <v>Uber</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F23" t="str">
         <v/>
       </c>
       <c r="G23" t="str">
-        <v>CARTAO_DEBITO</v>
+        <v>OUTRO</v>
       </c>
       <c r="H23">
-        <v>202</v>
-      </c>
-      <c r="I23">
-        <v>202</v>
+        <v>602</v>
+      </c>
+      <c r="I23" t="str">
+        <v/>
       </c>
       <c r="J23" t="str">
-        <v>Transporte/App</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K23" t="str">
-        <v>Transporte/App</v>
+        <v/>
       </c>
       <c r="L23" t="str">
-        <v>spend</v>
+        <v>income</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -1815,36 +1815,36 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23">
         <v>0</v>
       </c>
       <c r="R23" t="str">
-        <v>Palavra-chave 'UBER' identificada, classificado como Transporte/App.</v>
+        <v>Classificado como rendimento de investimento por descrição.</v>
       </c>
       <c r="S23">
-        <v>0.97</v>
+        <v>0.9</v>
       </c>
       <c r="T23" t="str">
-        <v>68a642d1-fead-48b9-aebf-c5f97d7d5e3c</v>
+        <v>1732529161827</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>2025-08-26</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B24" t="str">
-        <v>Pagamento de fatura</v>
+        <v>Dinheiro retirado Reserva</v>
       </c>
       <c r="C24">
-        <v>-52.93</v>
+        <v>245</v>
       </c>
       <c r="D24" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E24" t="str">
-        <v>Pagamento de fatura</v>
+        <v>Reserva</v>
       </c>
       <c r="F24" t="str">
         <v/>
@@ -1853,25 +1853,25 @@
         <v>OUTRO</v>
       </c>
       <c r="H24">
-        <v>502</v>
-      </c>
-      <c r="I24">
-        <v>502</v>
+        <v>603</v>
+      </c>
+      <c r="I24" t="str">
+        <v/>
       </c>
       <c r="J24" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v>Investimentos/Resgate</v>
       </c>
       <c r="K24" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v/>
       </c>
       <c r="L24" t="str">
-        <v>transfer</v>
+        <v>invest</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1883,30 +1883,30 @@
         <v>0</v>
       </c>
       <c r="R24" t="str">
-        <v>Prioridade 2: pagamento de fatura identificado. Não é gasto.</v>
+        <v>Resgate de reserva (retirada).</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="T24" t="str">
-        <v>68ae3f06-b81e-458e-ad35-f49e5acfa734</v>
+        <v>122401429670</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>2025-08-26</v>
+        <v>2025-08-14</v>
       </c>
       <c r="B25" t="str">
-        <v>Transferência recebida pelo Pix - Arthur Andrade Nunes - •••.908.292-•• - MERCADO PAGO IP LTDA. (0323) Agência: 1 Conta: 2807719770-6</v>
+        <v>Transferência Pix enviada Fred Williams de Oliveira Lima Junior</v>
       </c>
       <c r="C25">
-        <v>586.7</v>
+        <v>-245</v>
       </c>
       <c r="D25" t="str">
-        <v>credito</v>
+        <v>debito</v>
       </c>
       <c r="E25" t="str">
-        <v>Arthur Andrade Nunes</v>
+        <v>Fred Williams de Oliveira Lima Junior</v>
       </c>
       <c r="F25" t="str">
         <v/>
@@ -1915,22 +1915,22 @@
         <v>PIX</v>
       </c>
       <c r="H25">
-        <v>701</v>
-      </c>
-      <c r="I25">
-        <v>701</v>
+        <v>700</v>
+      </c>
+      <c r="I25" t="str">
+        <v/>
       </c>
       <c r="J25" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v>Transferências</v>
       </c>
       <c r="K25" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v/>
       </c>
       <c r="L25" t="str">
         <v>transfer</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -1945,30 +1945,30 @@
         <v>0</v>
       </c>
       <c r="R25" t="str">
-        <v>Prioridade 1: transferência interna identificada via nome titular.</v>
+        <v>Transferência Pix enviada para terceiro.</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="T25" t="str">
-        <v>68ae3f59-d9a8-4285-bd89-4f33c70466c6</v>
+        <v>121872608169</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>2025-08-26</v>
+        <v>2025-08-15</v>
       </c>
       <c r="B26" t="str">
-        <v>Pagamento de fatura</v>
+        <v>Rendimentos</v>
       </c>
       <c r="C26">
-        <v>-586.7</v>
+        <v>0.03</v>
       </c>
       <c r="D26" t="str">
-        <v>debito</v>
+        <v>credito</v>
       </c>
       <c r="E26" t="str">
-        <v>Pagamento de fatura</v>
+        <v>Rendimentos</v>
       </c>
       <c r="F26" t="str">
         <v/>
@@ -1977,55 +1977,1357 @@
         <v>OUTRO</v>
       </c>
       <c r="H26">
-        <v>502</v>
-      </c>
-      <c r="I26">
-        <v>502</v>
+        <v>602</v>
+      </c>
+      <c r="I26" t="str">
+        <v/>
       </c>
       <c r="J26" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="K26" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v/>
       </c>
       <c r="L26" t="str">
+        <v>income</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S26">
+        <v>0.9</v>
+      </c>
+      <c r="T26" t="str">
+        <v>1732567236943</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>2025-08-18</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C27">
+        <v>0.03</v>
+      </c>
+      <c r="D27" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+      <c r="G27" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H27">
+        <v>602</v>
+      </c>
+      <c r="I27" t="str">
+        <v/>
+      </c>
+      <c r="J27" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K27" t="str">
+        <v/>
+      </c>
+      <c r="L27" t="str">
+        <v>income</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S27">
+        <v>0.9</v>
+      </c>
+      <c r="T27" t="str">
+        <v>1732608634669</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>2025-08-19</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C28">
+        <v>0.03</v>
+      </c>
+      <c r="D28" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
+      <c r="G28" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H28">
+        <v>602</v>
+      </c>
+      <c r="I28" t="str">
+        <v/>
+      </c>
+      <c r="J28" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K28" t="str">
+        <v/>
+      </c>
+      <c r="L28" t="str">
+        <v>income</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S28">
+        <v>0.9</v>
+      </c>
+      <c r="T28" t="str">
+        <v>1732684514103</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>2025-08-20</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C29">
+        <v>0.03</v>
+      </c>
+      <c r="D29" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H29">
+        <v>602</v>
+      </c>
+      <c r="I29" t="str">
+        <v/>
+      </c>
+      <c r="J29" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K29" t="str">
+        <v/>
+      </c>
+      <c r="L29" t="str">
+        <v>income</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S29">
+        <v>0.9</v>
+      </c>
+      <c r="T29" t="str">
+        <v>1732737787190</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>2025-08-20</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Transferência Pix recebida Arthur Andrade Nunes</v>
+      </c>
+      <c r="C30">
+        <v>250</v>
+      </c>
+      <c r="D30" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Arthur Andrade Nunes</v>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+      <c r="G30" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H30">
+        <v>701</v>
+      </c>
+      <c r="I30" t="str">
+        <v/>
+      </c>
+      <c r="J30" t="str">
+        <v>Transferências/Interna (Movimentação bancária)</v>
+      </c>
+      <c r="K30" t="str">
+        <v/>
+      </c>
+      <c r="L30" t="str">
         <v>transfer</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26" t="str">
-        <v>Prioridade 2: pagamento de fatura identificado. Não é gasto.</v>
-      </c>
-      <c r="S26">
-        <v>1</v>
-      </c>
-      <c r="T26" t="str">
-        <v>68ae3f6c-7880-44ba-a47d-d3be1da21b3d</v>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30" t="str">
+        <v>Transferência recebida do titular; transferência interna.</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30" t="str">
+        <v>122512423195</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>2025-08-20</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Dinheiro reservado Reserva</v>
+      </c>
+      <c r="C31">
+        <v>-250</v>
+      </c>
+      <c r="D31" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Reserva</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H31">
+        <v>604</v>
+      </c>
+      <c r="I31" t="str">
+        <v/>
+      </c>
+      <c r="J31" t="str">
+        <v>Investimentos/Aplicação</v>
+      </c>
+      <c r="K31" t="str">
+        <v/>
+      </c>
+      <c r="L31" t="str">
+        <v>invest</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31" t="str">
+        <v>Aplicação em reserva (aporte/investimento).</v>
+      </c>
+      <c r="S31">
+        <v>0.95</v>
+      </c>
+      <c r="T31" t="str">
+        <v>122512012945</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>2025-08-20</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Pagamento com QR Pix CONSORCIO FENIX</v>
+      </c>
+      <c r="C32">
+        <v>-30</v>
+      </c>
+      <c r="D32" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E32" t="str">
+        <v>CONSORCIO FENIX</v>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+      <c r="G32" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H32">
+        <v>200</v>
+      </c>
+      <c r="I32">
+        <v>203</v>
+      </c>
+      <c r="J32" t="str">
+        <v>Transporte</v>
+      </c>
+      <c r="K32" t="str">
+        <v>Transporte/Onibus</v>
+      </c>
+      <c r="L32" t="str">
+        <v>spend</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32" t="str">
+        <v>Regra do usuário: Consorcio Fenix = Transporte/Ônibus.</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32" t="str">
+        <v>123073933882</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>2025-08-21</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C33">
+        <v>0.03</v>
+      </c>
+      <c r="D33" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H33">
+        <v>602</v>
+      </c>
+      <c r="I33" t="str">
+        <v/>
+      </c>
+      <c r="J33" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K33" t="str">
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <v>income</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S33">
+        <v>0.9</v>
+      </c>
+      <c r="T33" t="str">
+        <v>1732786332683</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>2025-08-22</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C34">
+        <v>0.02</v>
+      </c>
+      <c r="D34" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+      <c r="G34" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H34">
+        <v>602</v>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
+      <c r="J34" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K34" t="str">
+        <v/>
+      </c>
+      <c r="L34" t="str">
+        <v>income</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S34">
+        <v>0.9</v>
+      </c>
+      <c r="T34" t="str">
+        <v>1732839147330</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>2025-08-22</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Transferência Pix enviada EDUARDO PINHEIRO GUSMAO</v>
+      </c>
+      <c r="C35">
+        <v>-20</v>
+      </c>
+      <c r="D35" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E35" t="str">
+        <v>EDUARDO PINHEIRO GUSMAO</v>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H35">
+        <v>700</v>
+      </c>
+      <c r="I35" t="str">
+        <v/>
+      </c>
+      <c r="J35" t="str">
+        <v>Transferências</v>
+      </c>
+      <c r="K35" t="str">
+        <v/>
+      </c>
+      <c r="L35" t="str">
+        <v>transfer</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35" t="str">
+        <v>Transferência Pix enviada para terceiro.</v>
+      </c>
+      <c r="S35">
+        <v>0.9</v>
+      </c>
+      <c r="T35" t="str">
+        <v>123370597700</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>2025-08-25</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C36">
+        <v>0.02</v>
+      </c>
+      <c r="D36" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+      <c r="G36" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H36">
+        <v>602</v>
+      </c>
+      <c r="I36" t="str">
+        <v/>
+      </c>
+      <c r="J36" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K36" t="str">
+        <v/>
+      </c>
+      <c r="L36" t="str">
+        <v>income</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S36">
+        <v>0.9</v>
+      </c>
+      <c r="T36" t="str">
+        <v>1732882101876</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>2025-08-26</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C37">
+        <v>0.01</v>
+      </c>
+      <c r="D37" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+      <c r="G37" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H37">
+        <v>602</v>
+      </c>
+      <c r="I37" t="str">
+        <v/>
+      </c>
+      <c r="J37" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K37" t="str">
+        <v/>
+      </c>
+      <c r="L37" t="str">
+        <v>income</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S37">
+        <v>0.9</v>
+      </c>
+      <c r="T37" t="str">
+        <v>1732957204064</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>2025-08-26</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Dinheiro retirado Reserva</v>
+      </c>
+      <c r="C38">
+        <v>586.7</v>
+      </c>
+      <c r="D38" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Reserva</v>
+      </c>
+      <c r="F38" t="str">
+        <v/>
+      </c>
+      <c r="G38" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H38">
+        <v>603</v>
+      </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
+      <c r="J38" t="str">
+        <v>Investimentos/Resgate</v>
+      </c>
+      <c r="K38" t="str">
+        <v/>
+      </c>
+      <c r="L38" t="str">
+        <v>invest</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38" t="str">
+        <v>Resgate de reserva (retirada).</v>
+      </c>
+      <c r="S38">
+        <v>0.95</v>
+      </c>
+      <c r="T38" t="str">
+        <v>123794830706</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>2025-08-26</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Transferência Pix enviada Arthur Andrade Nunes</v>
+      </c>
+      <c r="C39">
+        <v>-586.7</v>
+      </c>
+      <c r="D39" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Arthur Andrade Nunes</v>
+      </c>
+      <c r="F39" t="str">
+        <v/>
+      </c>
+      <c r="G39" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H39">
+        <v>701</v>
+      </c>
+      <c r="I39" t="str">
+        <v/>
+      </c>
+      <c r="J39" t="str">
+        <v>Transferências/Interna (Movimentação bancária)</v>
+      </c>
+      <c r="K39" t="str">
+        <v/>
+      </c>
+      <c r="L39" t="str">
+        <v>transfer</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39" t="str">
+        <v>Transferência enviada do titular para própria conta (Arthur Andrade Nunes) — transferência interna.</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+      <c r="T39" t="str">
+        <v>123794882722</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>2025-08-27</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C40">
+        <v>0.01</v>
+      </c>
+      <c r="D40" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
+      <c r="G40" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H40">
+        <v>602</v>
+      </c>
+      <c r="I40" t="str">
+        <v/>
+      </c>
+      <c r="J40" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K40" t="str">
+        <v/>
+      </c>
+      <c r="L40" t="str">
+        <v>income</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S40">
+        <v>0.9</v>
+      </c>
+      <c r="T40" t="str">
+        <v>1733012964474</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>2025-08-28</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C41">
+        <v>0.01</v>
+      </c>
+      <c r="D41" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F41" t="str">
+        <v/>
+      </c>
+      <c r="G41" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H41">
+        <v>602</v>
+      </c>
+      <c r="I41" t="str">
+        <v/>
+      </c>
+      <c r="J41" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K41" t="str">
+        <v/>
+      </c>
+      <c r="L41" t="str">
+        <v>income</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S41">
+        <v>0.9</v>
+      </c>
+      <c r="T41" t="str">
+        <v>1733057289168</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>2025-08-28</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Dinheiro retirado Reserva</v>
+      </c>
+      <c r="C42">
+        <v>30</v>
+      </c>
+      <c r="D42" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Reserva</v>
+      </c>
+      <c r="F42" t="str">
+        <v/>
+      </c>
+      <c r="G42" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H42">
+        <v>603</v>
+      </c>
+      <c r="I42" t="str">
+        <v/>
+      </c>
+      <c r="J42" t="str">
+        <v>Investimentos/Resgate</v>
+      </c>
+      <c r="K42" t="str">
+        <v/>
+      </c>
+      <c r="L42" t="str">
+        <v>invest</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42" t="str">
+        <v>Resgate de reserva (retirada).</v>
+      </c>
+      <c r="S42">
+        <v>0.95</v>
+      </c>
+      <c r="T42" t="str">
+        <v>123964660752</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>2025-08-28</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Pagamento com QR Pix CONSORCIO FENIX</v>
+      </c>
+      <c r="C43">
+        <v>-30</v>
+      </c>
+      <c r="D43" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E43" t="str">
+        <v>CONSORCIO FENIX</v>
+      </c>
+      <c r="F43" t="str">
+        <v/>
+      </c>
+      <c r="G43" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H43">
+        <v>200</v>
+      </c>
+      <c r="I43">
+        <v>203</v>
+      </c>
+      <c r="J43" t="str">
+        <v>Transporte</v>
+      </c>
+      <c r="K43" t="str">
+        <v>Transporte/Onibus</v>
+      </c>
+      <c r="L43" t="str">
+        <v>spend</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43" t="str">
+        <v>Regra do usuário para CONSORCIO FENIX – Transporte/Ônibus.</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43" t="str">
+        <v>123964850300</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>2025-08-29</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="C44">
+        <v>0.01</v>
+      </c>
+      <c r="D44" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Rendimentos</v>
+      </c>
+      <c r="F44" t="str">
+        <v/>
+      </c>
+      <c r="G44" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H44">
+        <v>602</v>
+      </c>
+      <c r="I44" t="str">
+        <v/>
+      </c>
+      <c r="J44" t="str">
+        <v>Investimentos/Rendimentos</v>
+      </c>
+      <c r="K44" t="str">
+        <v/>
+      </c>
+      <c r="L44" t="str">
+        <v>income</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44" t="str">
+        <v>Classificado como rendimento de investimento por descrição.</v>
+      </c>
+      <c r="S44">
+        <v>0.9</v>
+      </c>
+      <c r="T44" t="str">
+        <v>1733117204573</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>2025-08-29</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Transferência Pix recebida Wise Brasil Corretora de CÃ¢mbio Ltda.</v>
+      </c>
+      <c r="C45">
+        <v>3123.65</v>
+      </c>
+      <c r="D45" t="str">
+        <v>credito</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Wise Brasil Corretora de Câmbio Ltda.</v>
+      </c>
+      <c r="F45" t="str">
+        <v/>
+      </c>
+      <c r="G45" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H45">
+        <v>800</v>
+      </c>
+      <c r="I45" t="str">
+        <v/>
+      </c>
+      <c r="J45" t="str">
+        <v>Renda/Salário</v>
+      </c>
+      <c r="K45" t="str">
+        <v/>
+      </c>
+      <c r="L45" t="str">
+        <v>income</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45" t="str">
+        <v>Regra do usuário para Wise Brasil Corretora de Câmbio Ltda. (salário).</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="T45" t="str">
+        <v>124097780722</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>2025-08-29</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Dinheiro reservado Reserva</v>
+      </c>
+      <c r="C46">
+        <v>-639.63</v>
+      </c>
+      <c r="D46" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Reserva</v>
+      </c>
+      <c r="F46" t="str">
+        <v/>
+      </c>
+      <c r="G46" t="str">
+        <v>OUTRO</v>
+      </c>
+      <c r="H46">
+        <v>604</v>
+      </c>
+      <c r="I46" t="str">
+        <v/>
+      </c>
+      <c r="J46" t="str">
+        <v>Investimentos/Aplicação</v>
+      </c>
+      <c r="K46" t="str">
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <v>invest</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46" t="str">
+        <v>Aplicação em reserva (aporte/investimento).</v>
+      </c>
+      <c r="S46">
+        <v>0.95</v>
+      </c>
+      <c r="T46" t="str">
+        <v>123558432103</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>2025-08-30</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Transferência Pix enviada Miria dos Reis Almeida</v>
+      </c>
+      <c r="C47">
+        <v>-21.46</v>
+      </c>
+      <c r="D47" t="str">
+        <v>debito</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Miria dos Reis Almeida</v>
+      </c>
+      <c r="F47" t="str">
+        <v/>
+      </c>
+      <c r="G47" t="str">
+        <v>PIX</v>
+      </c>
+      <c r="H47">
+        <v>700</v>
+      </c>
+      <c r="I47" t="str">
+        <v/>
+      </c>
+      <c r="J47" t="str">
+        <v>Transferências</v>
+      </c>
+      <c r="K47" t="str">
+        <v/>
+      </c>
+      <c r="L47" t="str">
+        <v>transfer</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47" t="str">
+        <v>Transferência Pix enviada para terceiro.</v>
+      </c>
+      <c r="S47">
+        <v>0.9</v>
+      </c>
+      <c r="T47" t="str">
+        <v>123740740781</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T47"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2049,120 +3351,153 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Transferências/Interna (Movimentação bancária)</v>
+        <v>Investimentos/Rendimentos</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>-230.18</v>
+        <v>2.46</v>
       </c>
       <c r="E2">
-        <v>-46.04</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Transferências</v>
+        <v>Renda/Salário</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>1174.75</v>
+        <v>6272.39</v>
       </c>
       <c r="E3">
-        <v>146.84</v>
+        <v>2090.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Alimentação/Supermercado</v>
+        <v>Transferências/Interna (Movimentação bancária)</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>-167.21</v>
+        <v>230.18</v>
       </c>
       <c r="E4">
-        <v>-167.21</v>
+        <v>46.04</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Serviços financeiros/Cartão – Pagamento de fatura</v>
+        <v>Moradia/Condomínio</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>-1761.43</v>
+        <v>-809.03</v>
       </c>
       <c r="E5">
-        <v>-587.14</v>
+        <v>-809.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Investimentos/Rendimentos</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Investimentos/Rendimentos</v>
+        <v>Moradia/Aluguel</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>8.25</v>
+        <v>-2378.2</v>
       </c>
       <c r="E6">
-        <v>1.38</v>
+        <v>-2378.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Outros/Diversos</v>
+        <v>Outros</v>
       </c>
       <c r="B7" t="str">
         <v>Outros/Diversos</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>-700</v>
+        <v>-280.76</v>
       </c>
       <c r="E7">
-        <v>-700</v>
+        <v>-140.38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Transporte/App</v>
+        <v>Transporte</v>
       </c>
       <c r="B8" t="str">
-        <v>Transporte/App</v>
+        <v>Transporte/Onibus</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>-6.86</v>
+        <v>-90</v>
       </c>
       <c r="E8">
-        <v>-6.86</v>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Transferências</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>-496.46</v>
+      </c>
+      <c r="E9">
+        <v>-99.29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Investimentos/Resgate</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>861.7</v>
+      </c>
+      <c r="E10">
+        <v>287.23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Investimentos/Aplicação</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>-889.63</v>
+      </c>
+      <c r="E11">
+        <v>-444.81</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2187,13 +3522,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2846.82</v>
+        <v>9030.55</v>
       </c>
       <c r="B2">
-        <v>874.07</v>
+        <v>4944.08</v>
       </c>
       <c r="C2">
-        <v>1972.75</v>
+        <v>4086.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>